<commit_message>
Se agregó en filltables e  inittables la variable de CH_RSSI
</commit_message>
<xml_diff>
--- a/RS Debug DataFrame.xlsx
+++ b/RS Debug DataFrame.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CASTI\Documents\UNAM\Tesis\Software\COLMENA-RobotSoftware\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438F1FCB-68E2-470B-9323-C3EF0E73CCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA4B0BF-1108-492C-8141-FC51FAF3382E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS - TTDM DBG" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="287">
   <si>
     <t>Header</t>
   </si>
@@ -872,13 +872,37 @@
   </si>
   <si>
     <t>N 11</t>
+  </si>
+  <si>
+    <t>CH TX</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>NC_counter</t>
+  </si>
+  <si>
+    <t>RSSI CH1</t>
+  </si>
+  <si>
+    <t>RSSI CH2</t>
+  </si>
+  <si>
+    <t>RSSI CH3</t>
+  </si>
+  <si>
+    <t>RSSI CH4</t>
+  </si>
+  <si>
+    <t>RSSI CH5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -985,8 +1009,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="28">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1146,6 +1178,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1371,7 +1409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1567,6 +1605,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1576,20 +1624,38 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1597,10 +1663,82 @@
     <xf numFmtId="0" fontId="1" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1609,90 +1747,6 @@
     <xf numFmtId="0" fontId="1" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1753,14 +1807,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2082,10 +2139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F5C418-6B51-4341-ABCF-BEE607F5CA2B}">
-  <dimension ref="A2:HX8"/>
+  <dimension ref="A2:ID8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BY1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="FJ9" sqref="FJ9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="GE1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="HM10" sqref="HM10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,25 +2167,25 @@
     <col min="185" max="185" width="13" customWidth="1"/>
     <col min="186" max="186" width="18.85546875" customWidth="1"/>
     <col min="187" max="202" width="2.42578125" customWidth="1"/>
-    <col min="203" max="226" width="4" customWidth="1"/>
-    <col min="227" max="232" width="7.42578125" customWidth="1"/>
+    <col min="203" max="232" width="4" customWidth="1"/>
+    <col min="233" max="238" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:232" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="102" t="s">
+    <row r="2" spans="1:238" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
     </row>
-    <row r="3" spans="1:232" s="14" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:238" s="14" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -2140,7 +2197,7 @@
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
     </row>
-    <row r="4" spans="1:232" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:238" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="37">
@@ -2815,224 +2872,242 @@
       <c r="HR4" s="37">
         <v>223</v>
       </c>
-      <c r="HS4" s="38" t="s">
+      <c r="HS4" s="37">
+        <v>224</v>
+      </c>
+      <c r="HT4" s="37">
+        <v>225</v>
+      </c>
+      <c r="HU4" s="37">
+        <v>226</v>
+      </c>
+      <c r="HV4" s="37">
+        <v>227</v>
+      </c>
+      <c r="HW4" s="37">
+        <v>228</v>
+      </c>
+      <c r="HX4" s="37">
+        <v>229</v>
+      </c>
+      <c r="HY4" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="HT4" s="38">
+      <c r="HZ4" s="38">
         <v>248</v>
       </c>
-      <c r="HU4" s="38">
+      <c r="IA4" s="38">
         <v>249</v>
       </c>
-      <c r="HV4" s="38">
+      <c r="IB4" s="38">
         <v>251</v>
       </c>
-      <c r="HW4" s="38">
+      <c r="IC4" s="38">
         <v>252</v>
       </c>
-      <c r="HX4" s="38">
+      <c r="ID4" s="38">
         <v>253</v>
       </c>
     </row>
-    <row r="5" spans="1:232" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:238" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="103" t="s">
+      <c r="C5" s="106" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="104"/>
-      <c r="N5" s="104"/>
-      <c r="O5" s="105" t="s">
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="107"/>
+      <c r="L5" s="107"/>
+      <c r="M5" s="107"/>
+      <c r="N5" s="107"/>
+      <c r="O5" s="108" t="s">
         <v>146</v>
       </c>
-      <c r="P5" s="105"/>
-      <c r="Q5" s="105"/>
-      <c r="R5" s="105"/>
-      <c r="S5" s="105"/>
-      <c r="T5" s="105"/>
-      <c r="U5" s="105"/>
-      <c r="V5" s="105"/>
-      <c r="W5" s="105"/>
-      <c r="X5" s="105"/>
-      <c r="Y5" s="105"/>
-      <c r="Z5" s="105"/>
-      <c r="AA5" s="105"/>
-      <c r="AB5" s="105"/>
-      <c r="AC5" s="105"/>
-      <c r="AD5" s="105"/>
-      <c r="AE5" s="105"/>
-      <c r="AF5" s="105"/>
-      <c r="AG5" s="105"/>
-      <c r="AH5" s="105"/>
-      <c r="AI5" s="105"/>
-      <c r="AJ5" s="105"/>
-      <c r="AK5" s="105"/>
-      <c r="AL5" s="105"/>
-      <c r="AM5" s="105"/>
-      <c r="AN5" s="105"/>
-      <c r="AO5" s="105"/>
-      <c r="AP5" s="105"/>
-      <c r="AQ5" s="105"/>
-      <c r="AR5" s="105"/>
-      <c r="AS5" s="105"/>
-      <c r="AT5" s="105"/>
-      <c r="AU5" s="105"/>
-      <c r="AV5" s="105"/>
-      <c r="AW5" s="105"/>
-      <c r="AX5" s="105"/>
-      <c r="AY5" s="105"/>
-      <c r="AZ5" s="105"/>
-      <c r="BA5" s="105"/>
-      <c r="BB5" s="105"/>
-      <c r="BC5" s="105"/>
-      <c r="BD5" s="105"/>
-      <c r="BE5" s="105"/>
-      <c r="BF5" s="105"/>
-      <c r="BG5" s="105"/>
-      <c r="BH5" s="105"/>
-      <c r="BI5" s="105"/>
-      <c r="BJ5" s="105"/>
-      <c r="BK5" s="105"/>
-      <c r="BL5" s="105"/>
-      <c r="BM5" s="105"/>
-      <c r="BN5" s="105"/>
-      <c r="BO5" s="105"/>
-      <c r="BP5" s="105"/>
-      <c r="BQ5" s="105"/>
-      <c r="BR5" s="105"/>
-      <c r="BS5" s="77" t="s">
+      <c r="P5" s="108"/>
+      <c r="Q5" s="108"/>
+      <c r="R5" s="108"/>
+      <c r="S5" s="108"/>
+      <c r="T5" s="108"/>
+      <c r="U5" s="108"/>
+      <c r="V5" s="108"/>
+      <c r="W5" s="108"/>
+      <c r="X5" s="108"/>
+      <c r="Y5" s="108"/>
+      <c r="Z5" s="108"/>
+      <c r="AA5" s="108"/>
+      <c r="AB5" s="108"/>
+      <c r="AC5" s="108"/>
+      <c r="AD5" s="108"/>
+      <c r="AE5" s="108"/>
+      <c r="AF5" s="108"/>
+      <c r="AG5" s="108"/>
+      <c r="AH5" s="108"/>
+      <c r="AI5" s="108"/>
+      <c r="AJ5" s="108"/>
+      <c r="AK5" s="108"/>
+      <c r="AL5" s="108"/>
+      <c r="AM5" s="108"/>
+      <c r="AN5" s="108"/>
+      <c r="AO5" s="108"/>
+      <c r="AP5" s="108"/>
+      <c r="AQ5" s="108"/>
+      <c r="AR5" s="108"/>
+      <c r="AS5" s="108"/>
+      <c r="AT5" s="108"/>
+      <c r="AU5" s="108"/>
+      <c r="AV5" s="108"/>
+      <c r="AW5" s="108"/>
+      <c r="AX5" s="108"/>
+      <c r="AY5" s="108"/>
+      <c r="AZ5" s="108"/>
+      <c r="BA5" s="108"/>
+      <c r="BB5" s="108"/>
+      <c r="BC5" s="108"/>
+      <c r="BD5" s="108"/>
+      <c r="BE5" s="108"/>
+      <c r="BF5" s="108"/>
+      <c r="BG5" s="108"/>
+      <c r="BH5" s="108"/>
+      <c r="BI5" s="108"/>
+      <c r="BJ5" s="108"/>
+      <c r="BK5" s="108"/>
+      <c r="BL5" s="108"/>
+      <c r="BM5" s="108"/>
+      <c r="BN5" s="108"/>
+      <c r="BO5" s="108"/>
+      <c r="BP5" s="108"/>
+      <c r="BQ5" s="108"/>
+      <c r="BR5" s="108"/>
+      <c r="BS5" s="87" t="s">
         <v>243</v>
       </c>
-      <c r="BT5" s="77"/>
-      <c r="BU5" s="77"/>
-      <c r="BV5" s="77"/>
-      <c r="BW5" s="77"/>
-      <c r="BX5" s="77"/>
-      <c r="BY5" s="77"/>
-      <c r="BZ5" s="77"/>
-      <c r="CA5" s="77"/>
-      <c r="CB5" s="77"/>
-      <c r="CC5" s="77"/>
-      <c r="CD5" s="77"/>
-      <c r="CE5" s="77"/>
-      <c r="CF5" s="77"/>
-      <c r="CG5" s="77"/>
-      <c r="CH5" s="77"/>
-      <c r="CI5" s="77"/>
-      <c r="CJ5" s="77"/>
-      <c r="CK5" s="77"/>
-      <c r="CL5" s="77"/>
-      <c r="CM5" s="77"/>
-      <c r="CN5" s="77"/>
-      <c r="CO5" s="77"/>
-      <c r="CP5" s="77"/>
-      <c r="CQ5" s="77"/>
-      <c r="CR5" s="77"/>
-      <c r="CS5" s="77"/>
-      <c r="CT5" s="77"/>
-      <c r="CU5" s="77"/>
-      <c r="CV5" s="77"/>
-      <c r="CW5" s="77"/>
-      <c r="CX5" s="77"/>
-      <c r="CY5" s="77"/>
-      <c r="CZ5" s="77"/>
-      <c r="DA5" s="77"/>
-      <c r="DB5" s="77"/>
-      <c r="DC5" s="77"/>
-      <c r="DD5" s="77"/>
-      <c r="DE5" s="77"/>
-      <c r="DF5" s="77"/>
-      <c r="DG5" s="77"/>
-      <c r="DH5" s="77"/>
-      <c r="DI5" s="77"/>
-      <c r="DJ5" s="77"/>
-      <c r="DK5" s="78" t="s">
+      <c r="BT5" s="87"/>
+      <c r="BU5" s="87"/>
+      <c r="BV5" s="87"/>
+      <c r="BW5" s="87"/>
+      <c r="BX5" s="87"/>
+      <c r="BY5" s="87"/>
+      <c r="BZ5" s="87"/>
+      <c r="CA5" s="87"/>
+      <c r="CB5" s="87"/>
+      <c r="CC5" s="87"/>
+      <c r="CD5" s="87"/>
+      <c r="CE5" s="87"/>
+      <c r="CF5" s="87"/>
+      <c r="CG5" s="87"/>
+      <c r="CH5" s="87"/>
+      <c r="CI5" s="87"/>
+      <c r="CJ5" s="87"/>
+      <c r="CK5" s="87"/>
+      <c r="CL5" s="87"/>
+      <c r="CM5" s="87"/>
+      <c r="CN5" s="87"/>
+      <c r="CO5" s="87"/>
+      <c r="CP5" s="87"/>
+      <c r="CQ5" s="87"/>
+      <c r="CR5" s="87"/>
+      <c r="CS5" s="87"/>
+      <c r="CT5" s="87"/>
+      <c r="CU5" s="87"/>
+      <c r="CV5" s="87"/>
+      <c r="CW5" s="87"/>
+      <c r="CX5" s="87"/>
+      <c r="CY5" s="87"/>
+      <c r="CZ5" s="87"/>
+      <c r="DA5" s="87"/>
+      <c r="DB5" s="87"/>
+      <c r="DC5" s="87"/>
+      <c r="DD5" s="87"/>
+      <c r="DE5" s="87"/>
+      <c r="DF5" s="87"/>
+      <c r="DG5" s="87"/>
+      <c r="DH5" s="87"/>
+      <c r="DI5" s="87"/>
+      <c r="DJ5" s="87"/>
+      <c r="DK5" s="88" t="s">
         <v>244</v>
       </c>
-      <c r="DL5" s="78"/>
-      <c r="DM5" s="78"/>
-      <c r="DN5" s="78"/>
-      <c r="DO5" s="78"/>
-      <c r="DP5" s="78"/>
-      <c r="DQ5" s="78"/>
-      <c r="DR5" s="78"/>
-      <c r="DS5" s="78"/>
-      <c r="DT5" s="78"/>
-      <c r="DU5" s="78"/>
-      <c r="DV5" s="78"/>
-      <c r="DW5" s="78"/>
-      <c r="DX5" s="78"/>
-      <c r="DY5" s="78"/>
-      <c r="DZ5" s="78"/>
-      <c r="EA5" s="78"/>
-      <c r="EB5" s="78"/>
-      <c r="EC5" s="78"/>
-      <c r="ED5" s="78"/>
-      <c r="EE5" s="78"/>
-      <c r="EF5" s="78"/>
-      <c r="EG5" s="78"/>
-      <c r="EH5" s="78"/>
-      <c r="EI5" s="78"/>
-      <c r="EJ5" s="78"/>
-      <c r="EK5" s="78"/>
-      <c r="EL5" s="78"/>
-      <c r="EM5" s="78"/>
-      <c r="EN5" s="78"/>
-      <c r="EO5" s="78"/>
-      <c r="EP5" s="78"/>
-      <c r="EQ5" s="78"/>
-      <c r="ER5" s="78"/>
-      <c r="ES5" s="78"/>
-      <c r="ET5" s="78"/>
-      <c r="EU5" s="78"/>
-      <c r="EV5" s="78"/>
-      <c r="EW5" s="78"/>
-      <c r="EX5" s="78"/>
-      <c r="EY5" s="78"/>
-      <c r="EZ5" s="78"/>
-      <c r="FA5" s="78"/>
-      <c r="FB5" s="78"/>
-      <c r="FC5" s="132" t="s">
+      <c r="DL5" s="88"/>
+      <c r="DM5" s="88"/>
+      <c r="DN5" s="88"/>
+      <c r="DO5" s="88"/>
+      <c r="DP5" s="88"/>
+      <c r="DQ5" s="88"/>
+      <c r="DR5" s="88"/>
+      <c r="DS5" s="88"/>
+      <c r="DT5" s="88"/>
+      <c r="DU5" s="88"/>
+      <c r="DV5" s="88"/>
+      <c r="DW5" s="88"/>
+      <c r="DX5" s="88"/>
+      <c r="DY5" s="88"/>
+      <c r="DZ5" s="88"/>
+      <c r="EA5" s="88"/>
+      <c r="EB5" s="88"/>
+      <c r="EC5" s="88"/>
+      <c r="ED5" s="88"/>
+      <c r="EE5" s="88"/>
+      <c r="EF5" s="88"/>
+      <c r="EG5" s="88"/>
+      <c r="EH5" s="88"/>
+      <c r="EI5" s="88"/>
+      <c r="EJ5" s="88"/>
+      <c r="EK5" s="88"/>
+      <c r="EL5" s="88"/>
+      <c r="EM5" s="88"/>
+      <c r="EN5" s="88"/>
+      <c r="EO5" s="88"/>
+      <c r="EP5" s="88"/>
+      <c r="EQ5" s="88"/>
+      <c r="ER5" s="88"/>
+      <c r="ES5" s="88"/>
+      <c r="ET5" s="88"/>
+      <c r="EU5" s="88"/>
+      <c r="EV5" s="88"/>
+      <c r="EW5" s="88"/>
+      <c r="EX5" s="88"/>
+      <c r="EY5" s="88"/>
+      <c r="EZ5" s="88"/>
+      <c r="FA5" s="88"/>
+      <c r="FB5" s="88"/>
+      <c r="FC5" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="FD5" s="132"/>
-      <c r="FE5" s="132"/>
-      <c r="FF5" s="132"/>
-      <c r="FG5" s="132"/>
-      <c r="FH5" s="132"/>
-      <c r="FI5" s="132"/>
-      <c r="FJ5" s="132"/>
-      <c r="FK5" s="132"/>
-      <c r="FL5" s="132"/>
-      <c r="FM5" s="132"/>
-      <c r="FN5" s="132"/>
-      <c r="FO5" s="106" t="s">
+      <c r="FD5" s="111"/>
+      <c r="FE5" s="111"/>
+      <c r="FF5" s="111"/>
+      <c r="FG5" s="111"/>
+      <c r="FH5" s="111"/>
+      <c r="FI5" s="111"/>
+      <c r="FJ5" s="111"/>
+      <c r="FK5" s="111"/>
+      <c r="FL5" s="111"/>
+      <c r="FM5" s="111"/>
+      <c r="FN5" s="111"/>
+      <c r="FO5" s="109" t="s">
         <v>158</v>
       </c>
-      <c r="FP5" s="107"/>
-      <c r="FQ5" s="107"/>
-      <c r="FR5" s="107"/>
-      <c r="FS5" s="107"/>
-      <c r="FT5" s="107"/>
-      <c r="FU5" s="107"/>
-      <c r="FV5" s="107"/>
-      <c r="FW5" s="107"/>
-      <c r="FX5" s="107"/>
-      <c r="FY5" s="107"/>
-      <c r="FZ5" s="107"/>
-      <c r="GA5" s="107"/>
-      <c r="GB5" s="107"/>
-      <c r="GC5" s="107"/>
-      <c r="GD5" s="107"/>
+      <c r="FP5" s="110"/>
+      <c r="FQ5" s="110"/>
+      <c r="FR5" s="110"/>
+      <c r="FS5" s="110"/>
+      <c r="FT5" s="110"/>
+      <c r="FU5" s="110"/>
+      <c r="FV5" s="110"/>
+      <c r="FW5" s="110"/>
+      <c r="FX5" s="110"/>
+      <c r="FY5" s="110"/>
+      <c r="FZ5" s="110"/>
+      <c r="GA5" s="110"/>
+      <c r="GB5" s="110"/>
+      <c r="GC5" s="110"/>
+      <c r="GD5" s="110"/>
       <c r="GE5" s="66"/>
       <c r="GF5" s="66"/>
       <c r="GG5" s="66"/>
@@ -3066,273 +3141,281 @@
       <c r="HG5" s="81" t="s">
         <v>209</v>
       </c>
-      <c r="HH5" s="82"/>
-      <c r="HI5" s="82"/>
-      <c r="HJ5" s="82"/>
-      <c r="HK5" s="82"/>
-      <c r="HL5" s="82"/>
-      <c r="HM5" s="82"/>
-      <c r="HN5" s="82"/>
-      <c r="HO5" s="82"/>
-      <c r="HP5" s="82"/>
-      <c r="HQ5" s="82"/>
-      <c r="HR5" s="82"/>
-      <c r="HS5" s="34"/>
-      <c r="HT5" s="34"/>
-      <c r="HU5" s="34"/>
-      <c r="HV5" s="91" t="s">
+      <c r="HH5" s="81"/>
+      <c r="HI5" s="81"/>
+      <c r="HJ5" s="81"/>
+      <c r="HK5" s="81"/>
+      <c r="HL5" s="81"/>
+      <c r="HM5" s="81"/>
+      <c r="HN5" s="81"/>
+      <c r="HO5" s="81"/>
+      <c r="HP5" s="81"/>
+      <c r="HQ5" s="81"/>
+      <c r="HR5" s="81"/>
+      <c r="HS5" s="137" t="s">
+        <v>280</v>
+      </c>
+      <c r="HT5" s="138"/>
+      <c r="HU5" s="138"/>
+      <c r="HV5" s="138"/>
+      <c r="HW5" s="138"/>
+      <c r="HX5" s="139"/>
+      <c r="HY5" s="72"/>
+      <c r="HZ5" s="34"/>
+      <c r="IA5" s="34"/>
+      <c r="IB5" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="HW5" s="92"/>
-      <c r="HX5" s="93"/>
+      <c r="IC5" s="90"/>
+      <c r="ID5" s="91"/>
     </row>
-    <row r="6" spans="1:232" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:238" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="96" t="s">
+      <c r="C6" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="97"/>
-      <c r="E6" s="98"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="96"/>
       <c r="F6" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="G6" s="74" t="s">
+      <c r="G6" s="76" t="s">
         <v>122</v>
       </c>
-      <c r="H6" s="76"/>
-      <c r="I6" s="74" t="s">
+      <c r="H6" s="78"/>
+      <c r="I6" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="J6" s="76"/>
-      <c r="K6" s="99" t="s">
+      <c r="J6" s="78"/>
+      <c r="K6" s="97" t="s">
         <v>125</v>
       </c>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="101"/>
-      <c r="O6" s="74" t="s">
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="99"/>
+      <c r="O6" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="74" t="s">
+      <c r="P6" s="78"/>
+      <c r="Q6" s="76" t="s">
         <v>132</v>
       </c>
-      <c r="R6" s="76"/>
-      <c r="S6" s="74" t="s">
+      <c r="R6" s="78"/>
+      <c r="S6" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="T6" s="75"/>
-      <c r="U6" s="75"/>
-      <c r="V6" s="76"/>
-      <c r="W6" s="74" t="s">
+      <c r="T6" s="77"/>
+      <c r="U6" s="77"/>
+      <c r="V6" s="78"/>
+      <c r="W6" s="76" t="s">
         <v>134</v>
       </c>
-      <c r="X6" s="75"/>
-      <c r="Y6" s="75"/>
-      <c r="Z6" s="76"/>
-      <c r="AA6" s="74" t="s">
+      <c r="X6" s="77"/>
+      <c r="Y6" s="77"/>
+      <c r="Z6" s="78"/>
+      <c r="AA6" s="76" t="s">
         <v>135</v>
       </c>
-      <c r="AB6" s="75"/>
-      <c r="AC6" s="75"/>
-      <c r="AD6" s="76"/>
-      <c r="AE6" s="74" t="s">
+      <c r="AB6" s="77"/>
+      <c r="AC6" s="77"/>
+      <c r="AD6" s="78"/>
+      <c r="AE6" s="76" t="s">
         <v>136</v>
       </c>
-      <c r="AF6" s="75"/>
-      <c r="AG6" s="75"/>
-      <c r="AH6" s="76"/>
-      <c r="AI6" s="74" t="s">
+      <c r="AF6" s="77"/>
+      <c r="AG6" s="77"/>
+      <c r="AH6" s="78"/>
+      <c r="AI6" s="76" t="s">
         <v>137</v>
       </c>
-      <c r="AJ6" s="75"/>
-      <c r="AK6" s="75"/>
-      <c r="AL6" s="76"/>
-      <c r="AM6" s="74" t="s">
+      <c r="AJ6" s="77"/>
+      <c r="AK6" s="77"/>
+      <c r="AL6" s="78"/>
+      <c r="AM6" s="76" t="s">
         <v>138</v>
       </c>
-      <c r="AN6" s="75"/>
-      <c r="AO6" s="75"/>
-      <c r="AP6" s="76"/>
-      <c r="AQ6" s="74" t="s">
+      <c r="AN6" s="77"/>
+      <c r="AO6" s="77"/>
+      <c r="AP6" s="78"/>
+      <c r="AQ6" s="76" t="s">
         <v>139</v>
       </c>
-      <c r="AR6" s="75"/>
-      <c r="AS6" s="75"/>
-      <c r="AT6" s="76"/>
-      <c r="AU6" s="74" t="s">
+      <c r="AR6" s="77"/>
+      <c r="AS6" s="77"/>
+      <c r="AT6" s="78"/>
+      <c r="AU6" s="76" t="s">
         <v>140</v>
       </c>
-      <c r="AV6" s="75"/>
-      <c r="AW6" s="75"/>
-      <c r="AX6" s="76"/>
-      <c r="AY6" s="74" t="s">
+      <c r="AV6" s="77"/>
+      <c r="AW6" s="77"/>
+      <c r="AX6" s="78"/>
+      <c r="AY6" s="76" t="s">
         <v>141</v>
       </c>
-      <c r="AZ6" s="75"/>
-      <c r="BA6" s="75"/>
-      <c r="BB6" s="76"/>
-      <c r="BC6" s="74" t="s">
+      <c r="AZ6" s="77"/>
+      <c r="BA6" s="77"/>
+      <c r="BB6" s="78"/>
+      <c r="BC6" s="76" t="s">
         <v>142</v>
       </c>
-      <c r="BD6" s="75"/>
-      <c r="BE6" s="75"/>
-      <c r="BF6" s="76"/>
-      <c r="BG6" s="74" t="s">
+      <c r="BD6" s="77"/>
+      <c r="BE6" s="77"/>
+      <c r="BF6" s="78"/>
+      <c r="BG6" s="76" t="s">
         <v>143</v>
       </c>
-      <c r="BH6" s="75"/>
-      <c r="BI6" s="75"/>
-      <c r="BJ6" s="76"/>
-      <c r="BK6" s="74" t="s">
+      <c r="BH6" s="77"/>
+      <c r="BI6" s="77"/>
+      <c r="BJ6" s="78"/>
+      <c r="BK6" s="76" t="s">
         <v>144</v>
       </c>
-      <c r="BL6" s="75"/>
-      <c r="BM6" s="75"/>
-      <c r="BN6" s="76"/>
-      <c r="BO6" s="74" t="s">
+      <c r="BL6" s="77"/>
+      <c r="BM6" s="77"/>
+      <c r="BN6" s="78"/>
+      <c r="BO6" s="76" t="s">
         <v>145</v>
       </c>
-      <c r="BP6" s="76"/>
-      <c r="BQ6" s="74" t="s">
+      <c r="BP6" s="78"/>
+      <c r="BQ6" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="BR6" s="76"/>
-      <c r="BS6" s="74" t="s">
+      <c r="BR6" s="78"/>
+      <c r="BS6" s="76" t="s">
         <v>245</v>
       </c>
-      <c r="BT6" s="75"/>
-      <c r="BU6" s="75"/>
-      <c r="BV6" s="76"/>
-      <c r="BW6" s="74" t="s">
+      <c r="BT6" s="77"/>
+      <c r="BU6" s="77"/>
+      <c r="BV6" s="78"/>
+      <c r="BW6" s="76" t="s">
         <v>246</v>
       </c>
-      <c r="BX6" s="75"/>
-      <c r="BY6" s="75"/>
-      <c r="BZ6" s="76"/>
-      <c r="CA6" s="74" t="s">
+      <c r="BX6" s="77"/>
+      <c r="BY6" s="77"/>
+      <c r="BZ6" s="78"/>
+      <c r="CA6" s="76" t="s">
         <v>247</v>
       </c>
-      <c r="CB6" s="75"/>
-      <c r="CC6" s="75"/>
-      <c r="CD6" s="76"/>
-      <c r="CE6" s="74" t="s">
+      <c r="CB6" s="77"/>
+      <c r="CC6" s="77"/>
+      <c r="CD6" s="78"/>
+      <c r="CE6" s="76" t="s">
         <v>248</v>
       </c>
-      <c r="CF6" s="75"/>
-      <c r="CG6" s="75"/>
-      <c r="CH6" s="76"/>
-      <c r="CI6" s="74" t="s">
+      <c r="CF6" s="77"/>
+      <c r="CG6" s="77"/>
+      <c r="CH6" s="78"/>
+      <c r="CI6" s="76" t="s">
         <v>249</v>
       </c>
-      <c r="CJ6" s="75"/>
-      <c r="CK6" s="75"/>
-      <c r="CL6" s="76"/>
-      <c r="CM6" s="74" t="s">
+      <c r="CJ6" s="77"/>
+      <c r="CK6" s="77"/>
+      <c r="CL6" s="78"/>
+      <c r="CM6" s="76" t="s">
         <v>250</v>
       </c>
-      <c r="CN6" s="75"/>
-      <c r="CO6" s="75"/>
-      <c r="CP6" s="76"/>
-      <c r="CQ6" s="74" t="s">
+      <c r="CN6" s="77"/>
+      <c r="CO6" s="77"/>
+      <c r="CP6" s="78"/>
+      <c r="CQ6" s="76" t="s">
         <v>251</v>
       </c>
-      <c r="CR6" s="75"/>
-      <c r="CS6" s="75"/>
-      <c r="CT6" s="76"/>
-      <c r="CU6" s="74" t="s">
+      <c r="CR6" s="77"/>
+      <c r="CS6" s="77"/>
+      <c r="CT6" s="78"/>
+      <c r="CU6" s="76" t="s">
         <v>252</v>
       </c>
-      <c r="CV6" s="75"/>
-      <c r="CW6" s="75"/>
-      <c r="CX6" s="76"/>
-      <c r="CY6" s="74" t="s">
+      <c r="CV6" s="77"/>
+      <c r="CW6" s="77"/>
+      <c r="CX6" s="78"/>
+      <c r="CY6" s="76" t="s">
         <v>253</v>
       </c>
-      <c r="CZ6" s="75"/>
-      <c r="DA6" s="75"/>
-      <c r="DB6" s="76"/>
-      <c r="DC6" s="74" t="s">
+      <c r="CZ6" s="77"/>
+      <c r="DA6" s="77"/>
+      <c r="DB6" s="78"/>
+      <c r="DC6" s="76" t="s">
         <v>254</v>
       </c>
-      <c r="DD6" s="75"/>
-      <c r="DE6" s="75"/>
-      <c r="DF6" s="76"/>
-      <c r="DG6" s="74" t="s">
+      <c r="DD6" s="77"/>
+      <c r="DE6" s="77"/>
+      <c r="DF6" s="78"/>
+      <c r="DG6" s="76" t="s">
         <v>255</v>
       </c>
-      <c r="DH6" s="75"/>
-      <c r="DI6" s="75"/>
-      <c r="DJ6" s="76"/>
-      <c r="DK6" s="74" t="s">
+      <c r="DH6" s="77"/>
+      <c r="DI6" s="77"/>
+      <c r="DJ6" s="78"/>
+      <c r="DK6" s="76" t="s">
         <v>256</v>
       </c>
-      <c r="DL6" s="75"/>
-      <c r="DM6" s="75"/>
-      <c r="DN6" s="76"/>
-      <c r="DO6" s="74" t="s">
+      <c r="DL6" s="77"/>
+      <c r="DM6" s="77"/>
+      <c r="DN6" s="78"/>
+      <c r="DO6" s="76" t="s">
         <v>257</v>
       </c>
-      <c r="DP6" s="75"/>
-      <c r="DQ6" s="75"/>
-      <c r="DR6" s="76"/>
-      <c r="DS6" s="74" t="s">
+      <c r="DP6" s="77"/>
+      <c r="DQ6" s="77"/>
+      <c r="DR6" s="78"/>
+      <c r="DS6" s="76" t="s">
         <v>258</v>
       </c>
-      <c r="DT6" s="75"/>
-      <c r="DU6" s="75"/>
-      <c r="DV6" s="76"/>
-      <c r="DW6" s="74" t="s">
+      <c r="DT6" s="77"/>
+      <c r="DU6" s="77"/>
+      <c r="DV6" s="78"/>
+      <c r="DW6" s="76" t="s">
         <v>259</v>
       </c>
-      <c r="DX6" s="75"/>
-      <c r="DY6" s="75"/>
-      <c r="DZ6" s="76"/>
-      <c r="EA6" s="74" t="s">
+      <c r="DX6" s="77"/>
+      <c r="DY6" s="77"/>
+      <c r="DZ6" s="78"/>
+      <c r="EA6" s="76" t="s">
         <v>260</v>
       </c>
-      <c r="EB6" s="75"/>
-      <c r="EC6" s="75"/>
-      <c r="ED6" s="76"/>
-      <c r="EE6" s="74" t="s">
+      <c r="EB6" s="77"/>
+      <c r="EC6" s="77"/>
+      <c r="ED6" s="78"/>
+      <c r="EE6" s="76" t="s">
         <v>261</v>
       </c>
-      <c r="EF6" s="75"/>
-      <c r="EG6" s="75"/>
-      <c r="EH6" s="76"/>
-      <c r="EI6" s="74" t="s">
+      <c r="EF6" s="77"/>
+      <c r="EG6" s="77"/>
+      <c r="EH6" s="78"/>
+      <c r="EI6" s="76" t="s">
         <v>262</v>
       </c>
-      <c r="EJ6" s="75"/>
-      <c r="EK6" s="75"/>
-      <c r="EL6" s="76"/>
-      <c r="EM6" s="74" t="s">
+      <c r="EJ6" s="77"/>
+      <c r="EK6" s="77"/>
+      <c r="EL6" s="78"/>
+      <c r="EM6" s="76" t="s">
         <v>263</v>
       </c>
-      <c r="EN6" s="75"/>
-      <c r="EO6" s="75"/>
-      <c r="EP6" s="76"/>
-      <c r="EQ6" s="74" t="s">
+      <c r="EN6" s="77"/>
+      <c r="EO6" s="77"/>
+      <c r="EP6" s="78"/>
+      <c r="EQ6" s="76" t="s">
         <v>264</v>
       </c>
-      <c r="ER6" s="75"/>
-      <c r="ES6" s="75"/>
-      <c r="ET6" s="76"/>
-      <c r="EU6" s="74" t="s">
+      <c r="ER6" s="77"/>
+      <c r="ES6" s="77"/>
+      <c r="ET6" s="78"/>
+      <c r="EU6" s="76" t="s">
         <v>265</v>
       </c>
-      <c r="EV6" s="75"/>
-      <c r="EW6" s="75"/>
-      <c r="EX6" s="76"/>
-      <c r="EY6" s="74" t="s">
+      <c r="EV6" s="77"/>
+      <c r="EW6" s="77"/>
+      <c r="EX6" s="78"/>
+      <c r="EY6" s="76" t="s">
         <v>266</v>
       </c>
-      <c r="EZ6" s="75"/>
-      <c r="FA6" s="75"/>
-      <c r="FB6" s="76"/>
+      <c r="EZ6" s="77"/>
+      <c r="FA6" s="77"/>
+      <c r="FB6" s="78"/>
       <c r="FC6" s="44" t="s">
         <v>268</v>
       </c>
@@ -3369,22 +3452,22 @@
       <c r="FN6" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="FO6" s="86" t="s">
+      <c r="FO6" s="100" t="s">
         <v>149</v>
       </c>
-      <c r="FP6" s="90"/>
-      <c r="FQ6" s="90"/>
-      <c r="FR6" s="87"/>
-      <c r="FS6" s="86" t="s">
+      <c r="FP6" s="104"/>
+      <c r="FQ6" s="104"/>
+      <c r="FR6" s="101"/>
+      <c r="FS6" s="100" t="s">
         <v>150</v>
       </c>
-      <c r="FT6" s="90"/>
-      <c r="FU6" s="90"/>
-      <c r="FV6" s="87"/>
-      <c r="FW6" s="86" t="s">
+      <c r="FT6" s="104"/>
+      <c r="FU6" s="104"/>
+      <c r="FV6" s="101"/>
+      <c r="FW6" s="100" t="s">
         <v>151</v>
       </c>
-      <c r="FX6" s="87"/>
+      <c r="FX6" s="101"/>
       <c r="FY6" s="40" t="s">
         <v>152</v>
       </c>
@@ -3392,7 +3475,7 @@
         <v>153</v>
       </c>
       <c r="GA6" s="40" t="s">
-        <v>216</v>
+        <v>281</v>
       </c>
       <c r="GB6" s="40" t="s">
         <v>217</v>
@@ -3403,30 +3486,30 @@
       <c r="GD6" s="40" t="s">
         <v>219</v>
       </c>
-      <c r="GE6" s="74" t="s">
+      <c r="GE6" s="76" t="s">
         <v>212</v>
       </c>
-      <c r="GF6" s="75"/>
-      <c r="GG6" s="75"/>
-      <c r="GH6" s="76"/>
-      <c r="GI6" s="74" t="s">
+      <c r="GF6" s="77"/>
+      <c r="GG6" s="77"/>
+      <c r="GH6" s="78"/>
+      <c r="GI6" s="76" t="s">
         <v>213</v>
       </c>
-      <c r="GJ6" s="75"/>
-      <c r="GK6" s="75"/>
-      <c r="GL6" s="76"/>
-      <c r="GM6" s="74" t="s">
+      <c r="GJ6" s="77"/>
+      <c r="GK6" s="77"/>
+      <c r="GL6" s="78"/>
+      <c r="GM6" s="76" t="s">
         <v>214</v>
       </c>
-      <c r="GN6" s="75"/>
-      <c r="GO6" s="75"/>
-      <c r="GP6" s="76"/>
-      <c r="GQ6" s="74" t="s">
+      <c r="GN6" s="77"/>
+      <c r="GO6" s="77"/>
+      <c r="GP6" s="78"/>
+      <c r="GQ6" s="76" t="s">
         <v>215</v>
       </c>
-      <c r="GR6" s="75"/>
-      <c r="GS6" s="75"/>
-      <c r="GT6" s="76"/>
+      <c r="GR6" s="77"/>
+      <c r="GS6" s="77"/>
+      <c r="GT6" s="78"/>
       <c r="GU6" s="50" t="s">
         <v>231</v>
       </c>
@@ -3499,26 +3582,44 @@
       <c r="HR6" s="52" t="s">
         <v>242</v>
       </c>
-      <c r="HS6" s="67" t="s">
+      <c r="HS6" s="71" t="s">
+        <v>279</v>
+      </c>
+      <c r="HT6" s="140" t="s">
+        <v>282</v>
+      </c>
+      <c r="HU6" s="140" t="s">
+        <v>283</v>
+      </c>
+      <c r="HV6" s="140" t="s">
+        <v>284</v>
+      </c>
+      <c r="HW6" s="140" t="s">
+        <v>285</v>
+      </c>
+      <c r="HX6" s="140" t="s">
+        <v>286</v>
+      </c>
+      <c r="HY6" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="HT6" s="67" t="s">
+      <c r="HZ6" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="HU6" s="67" t="s">
+      <c r="IA6" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="HV6" s="26" t="s">
+      <c r="IB6" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="HW6" s="88" t="s">
+      <c r="IC6" s="102" t="s">
         <v>210</v>
       </c>
-      <c r="HX6" s="89"/>
+      <c r="ID6" s="103"/>
     </row>
-    <row r="7" spans="1:232" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:238" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="95"/>
+      <c r="B7" s="93"/>
       <c r="C7" s="20" t="s">
         <v>117</v>
       </c>
@@ -3531,244 +3632,244 @@
       <c r="F7" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="G7" s="72" t="s">
+      <c r="G7" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="H7" s="73"/>
+      <c r="H7" s="83"/>
       <c r="I7" s="68" t="s">
         <v>72</v>
       </c>
       <c r="J7" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="K7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="L7" s="70"/>
-      <c r="M7" s="70"/>
-      <c r="N7" s="71"/>
-      <c r="O7" s="72" t="s">
+      <c r="K7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="72" t="s">
+      <c r="P7" s="83"/>
+      <c r="Q7" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="R7" s="73"/>
-      <c r="S7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="T7" s="70"/>
-      <c r="U7" s="70"/>
-      <c r="V7" s="71"/>
-      <c r="W7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="X7" s="70"/>
-      <c r="Y7" s="70"/>
-      <c r="Z7" s="71"/>
-      <c r="AA7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB7" s="70"/>
-      <c r="AC7" s="70"/>
-      <c r="AD7" s="71"/>
-      <c r="AE7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="AF7" s="70"/>
-      <c r="AG7" s="70"/>
-      <c r="AH7" s="71"/>
-      <c r="AI7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="AJ7" s="70"/>
-      <c r="AK7" s="70"/>
-      <c r="AL7" s="71"/>
-      <c r="AM7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="AN7" s="70"/>
-      <c r="AO7" s="70"/>
-      <c r="AP7" s="71"/>
-      <c r="AQ7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="AR7" s="70"/>
-      <c r="AS7" s="70"/>
-      <c r="AT7" s="71"/>
-      <c r="AU7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="AV7" s="70"/>
-      <c r="AW7" s="70"/>
-      <c r="AX7" s="71"/>
-      <c r="AY7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="AZ7" s="70"/>
-      <c r="BA7" s="70"/>
-      <c r="BB7" s="71"/>
-      <c r="BC7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="BD7" s="70"/>
-      <c r="BE7" s="70"/>
-      <c r="BF7" s="71"/>
-      <c r="BG7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="BH7" s="70"/>
-      <c r="BI7" s="70"/>
-      <c r="BJ7" s="71"/>
-      <c r="BK7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="BL7" s="70"/>
-      <c r="BM7" s="70"/>
-      <c r="BN7" s="71"/>
-      <c r="BO7" s="72" t="s">
+      <c r="R7" s="83"/>
+      <c r="S7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="T7" s="74"/>
+      <c r="U7" s="74"/>
+      <c r="V7" s="75"/>
+      <c r="W7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="X7" s="74"/>
+      <c r="Y7" s="74"/>
+      <c r="Z7" s="75"/>
+      <c r="AA7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB7" s="74"/>
+      <c r="AC7" s="74"/>
+      <c r="AD7" s="75"/>
+      <c r="AE7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF7" s="74"/>
+      <c r="AG7" s="74"/>
+      <c r="AH7" s="75"/>
+      <c r="AI7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="AJ7" s="74"/>
+      <c r="AK7" s="74"/>
+      <c r="AL7" s="75"/>
+      <c r="AM7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="AN7" s="74"/>
+      <c r="AO7" s="74"/>
+      <c r="AP7" s="75"/>
+      <c r="AQ7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="AR7" s="74"/>
+      <c r="AS7" s="74"/>
+      <c r="AT7" s="75"/>
+      <c r="AU7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="AV7" s="74"/>
+      <c r="AW7" s="74"/>
+      <c r="AX7" s="75"/>
+      <c r="AY7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="AZ7" s="74"/>
+      <c r="BA7" s="74"/>
+      <c r="BB7" s="75"/>
+      <c r="BC7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="BD7" s="74"/>
+      <c r="BE7" s="74"/>
+      <c r="BF7" s="75"/>
+      <c r="BG7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="BH7" s="74"/>
+      <c r="BI7" s="74"/>
+      <c r="BJ7" s="75"/>
+      <c r="BK7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="BL7" s="74"/>
+      <c r="BM7" s="74"/>
+      <c r="BN7" s="75"/>
+      <c r="BO7" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="BP7" s="73"/>
-      <c r="BQ7" s="131" t="s">
-        <v>72</v>
-      </c>
-      <c r="BR7" s="131" t="s">
-        <v>72</v>
-      </c>
-      <c r="BS7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="BT7" s="70"/>
-      <c r="BU7" s="70"/>
-      <c r="BV7" s="71"/>
-      <c r="BW7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="BX7" s="70"/>
-      <c r="BY7" s="70"/>
-      <c r="BZ7" s="71"/>
-      <c r="CA7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CB7" s="70"/>
-      <c r="CC7" s="70"/>
-      <c r="CD7" s="71"/>
-      <c r="CE7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CF7" s="70"/>
-      <c r="CG7" s="70"/>
-      <c r="CH7" s="71"/>
-      <c r="CI7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CJ7" s="70"/>
-      <c r="CK7" s="70"/>
-      <c r="CL7" s="71"/>
-      <c r="CM7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CN7" s="70"/>
-      <c r="CO7" s="70"/>
-      <c r="CP7" s="71"/>
-      <c r="CQ7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CR7" s="70"/>
-      <c r="CS7" s="70"/>
-      <c r="CT7" s="71"/>
-      <c r="CU7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CV7" s="70"/>
-      <c r="CW7" s="70"/>
-      <c r="CX7" s="71"/>
-      <c r="CY7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CZ7" s="70"/>
-      <c r="DA7" s="70"/>
-      <c r="DB7" s="71"/>
-      <c r="DC7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DD7" s="70"/>
-      <c r="DE7" s="70"/>
-      <c r="DF7" s="71"/>
-      <c r="DG7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DH7" s="70"/>
-      <c r="DI7" s="70"/>
-      <c r="DJ7" s="71"/>
-      <c r="DK7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DL7" s="70"/>
-      <c r="DM7" s="70"/>
-      <c r="DN7" s="71"/>
-      <c r="DO7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DP7" s="70"/>
-      <c r="DQ7" s="70"/>
-      <c r="DR7" s="71"/>
-      <c r="DS7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT7" s="70"/>
-      <c r="DU7" s="70"/>
-      <c r="DV7" s="71"/>
-      <c r="DW7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DX7" s="70"/>
-      <c r="DY7" s="70"/>
-      <c r="DZ7" s="71"/>
-      <c r="EA7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EB7" s="70"/>
-      <c r="EC7" s="70"/>
-      <c r="ED7" s="71"/>
-      <c r="EE7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EF7" s="70"/>
-      <c r="EG7" s="70"/>
-      <c r="EH7" s="71"/>
-      <c r="EI7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EJ7" s="70"/>
-      <c r="EK7" s="70"/>
-      <c r="EL7" s="71"/>
-      <c r="EM7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EN7" s="70"/>
-      <c r="EO7" s="70"/>
-      <c r="EP7" s="71"/>
-      <c r="EQ7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="ER7" s="70"/>
-      <c r="ES7" s="70"/>
-      <c r="ET7" s="71"/>
-      <c r="EU7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EV7" s="70"/>
-      <c r="EW7" s="70"/>
-      <c r="EX7" s="71"/>
-      <c r="EY7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EZ7" s="70"/>
-      <c r="FA7" s="70"/>
-      <c r="FB7" s="71"/>
+      <c r="BP7" s="83"/>
+      <c r="BQ7" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="BR7" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="BS7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="BT7" s="74"/>
+      <c r="BU7" s="74"/>
+      <c r="BV7" s="75"/>
+      <c r="BW7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="BX7" s="74"/>
+      <c r="BY7" s="74"/>
+      <c r="BZ7" s="75"/>
+      <c r="CA7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CB7" s="74"/>
+      <c r="CC7" s="74"/>
+      <c r="CD7" s="75"/>
+      <c r="CE7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CF7" s="74"/>
+      <c r="CG7" s="74"/>
+      <c r="CH7" s="75"/>
+      <c r="CI7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CJ7" s="74"/>
+      <c r="CK7" s="74"/>
+      <c r="CL7" s="75"/>
+      <c r="CM7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CN7" s="74"/>
+      <c r="CO7" s="74"/>
+      <c r="CP7" s="75"/>
+      <c r="CQ7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CR7" s="74"/>
+      <c r="CS7" s="74"/>
+      <c r="CT7" s="75"/>
+      <c r="CU7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CV7" s="74"/>
+      <c r="CW7" s="74"/>
+      <c r="CX7" s="75"/>
+      <c r="CY7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CZ7" s="74"/>
+      <c r="DA7" s="74"/>
+      <c r="DB7" s="75"/>
+      <c r="DC7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DD7" s="74"/>
+      <c r="DE7" s="74"/>
+      <c r="DF7" s="75"/>
+      <c r="DG7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DH7" s="74"/>
+      <c r="DI7" s="74"/>
+      <c r="DJ7" s="75"/>
+      <c r="DK7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL7" s="74"/>
+      <c r="DM7" s="74"/>
+      <c r="DN7" s="75"/>
+      <c r="DO7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DP7" s="74"/>
+      <c r="DQ7" s="74"/>
+      <c r="DR7" s="75"/>
+      <c r="DS7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DT7" s="74"/>
+      <c r="DU7" s="74"/>
+      <c r="DV7" s="75"/>
+      <c r="DW7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DX7" s="74"/>
+      <c r="DY7" s="74"/>
+      <c r="DZ7" s="75"/>
+      <c r="EA7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EB7" s="74"/>
+      <c r="EC7" s="74"/>
+      <c r="ED7" s="75"/>
+      <c r="EE7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EF7" s="74"/>
+      <c r="EG7" s="74"/>
+      <c r="EH7" s="75"/>
+      <c r="EI7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EJ7" s="74"/>
+      <c r="EK7" s="74"/>
+      <c r="EL7" s="75"/>
+      <c r="EM7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EN7" s="74"/>
+      <c r="EO7" s="74"/>
+      <c r="EP7" s="75"/>
+      <c r="EQ7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="ER7" s="74"/>
+      <c r="ES7" s="74"/>
+      <c r="ET7" s="75"/>
+      <c r="EU7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EV7" s="74"/>
+      <c r="EW7" s="74"/>
+      <c r="EX7" s="75"/>
+      <c r="EY7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EZ7" s="74"/>
+      <c r="FA7" s="74"/>
+      <c r="FB7" s="75"/>
       <c r="FC7" s="35" t="s">
         <v>208</v>
       </c>
@@ -3802,25 +3903,25 @@
       <c r="FM7" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="FN7" s="133" t="s">
-        <v>72</v>
-      </c>
-      <c r="FO7" s="83" t="s">
+      <c r="FN7" s="70" t="s">
+        <v>72</v>
+      </c>
+      <c r="FO7" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="FP7" s="84"/>
-      <c r="FQ7" s="84"/>
-      <c r="FR7" s="85"/>
-      <c r="FS7" s="83" t="s">
+      <c r="FP7" s="85"/>
+      <c r="FQ7" s="85"/>
+      <c r="FR7" s="86"/>
+      <c r="FS7" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="FT7" s="84"/>
-      <c r="FU7" s="84"/>
-      <c r="FV7" s="85"/>
-      <c r="FW7" s="72" t="s">
+      <c r="FT7" s="85"/>
+      <c r="FU7" s="85"/>
+      <c r="FV7" s="86"/>
+      <c r="FW7" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="FX7" s="73"/>
+      <c r="FX7" s="83"/>
       <c r="FY7" s="35" t="s">
         <v>128</v>
       </c>
@@ -3839,30 +3940,30 @@
       <c r="GD7" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="GE7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="GF7" s="70"/>
-      <c r="GG7" s="70"/>
-      <c r="GH7" s="71"/>
-      <c r="GI7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="GJ7" s="70"/>
-      <c r="GK7" s="70"/>
-      <c r="GL7" s="71"/>
-      <c r="GM7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="GN7" s="70"/>
-      <c r="GO7" s="70"/>
-      <c r="GP7" s="71"/>
-      <c r="GQ7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="GR7" s="70"/>
-      <c r="GS7" s="70"/>
-      <c r="GT7" s="71"/>
+      <c r="GE7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="GF7" s="74"/>
+      <c r="GG7" s="74"/>
+      <c r="GH7" s="75"/>
+      <c r="GI7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="GJ7" s="74"/>
+      <c r="GK7" s="74"/>
+      <c r="GL7" s="75"/>
+      <c r="GM7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="GN7" s="74"/>
+      <c r="GO7" s="74"/>
+      <c r="GP7" s="75"/>
+      <c r="GQ7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="GR7" s="74"/>
+      <c r="GS7" s="74"/>
+      <c r="GT7" s="75"/>
       <c r="GU7" s="35" t="s">
         <v>208</v>
       </c>
@@ -3935,24 +4036,42 @@
       <c r="HR7" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="HS7" s="3" t="s">
+      <c r="HS7" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="HT7" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="HU7" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="HV7" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="HW7" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="HX7" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="HY7" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="HT7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="HU7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="HV7" s="4" t="s">
+      <c r="HZ7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="IA7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="IB7" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="HW7" s="72" t="s">
+      <c r="IC7" s="82" t="s">
         <v>211</v>
       </c>
-      <c r="HX7" s="73"/>
+      <c r="ID7" s="83"/>
     </row>
-    <row r="8" spans="1:232" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:238" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3965,7 +4084,8 @@
       <c r="J8" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="109">
+  <mergeCells count="110">
+    <mergeCell ref="HS5:HX5"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="K5:N5"/>
@@ -3979,7 +4099,18 @@
     <mergeCell ref="W6:Z6"/>
     <mergeCell ref="AA6:AD6"/>
     <mergeCell ref="AE6:AH6"/>
-    <mergeCell ref="HV5:HX5"/>
+    <mergeCell ref="DG6:DJ6"/>
+    <mergeCell ref="AI6:AL6"/>
+    <mergeCell ref="AM6:AP6"/>
+    <mergeCell ref="AQ6:AT6"/>
+    <mergeCell ref="AU6:AX6"/>
+    <mergeCell ref="AY6:BB6"/>
+    <mergeCell ref="CQ6:CT6"/>
+    <mergeCell ref="EI6:EL6"/>
+    <mergeCell ref="EM6:EP6"/>
+    <mergeCell ref="EQ6:ET6"/>
+    <mergeCell ref="EU6:EX6"/>
+    <mergeCell ref="IB5:ID5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="G6:H6"/>
@@ -3993,7 +4124,7 @@
     <mergeCell ref="GI6:GL6"/>
     <mergeCell ref="GM6:GP6"/>
     <mergeCell ref="GQ6:GT6"/>
-    <mergeCell ref="HW6:HX6"/>
+    <mergeCell ref="IC6:ID6"/>
     <mergeCell ref="BG6:BJ6"/>
     <mergeCell ref="BK6:BN6"/>
     <mergeCell ref="BO6:BP6"/>
@@ -4003,12 +4134,7 @@
     <mergeCell ref="CU6:CX6"/>
     <mergeCell ref="CY6:DB6"/>
     <mergeCell ref="DC6:DF6"/>
-    <mergeCell ref="DG6:DJ6"/>
-    <mergeCell ref="AI6:AL6"/>
-    <mergeCell ref="AM6:AP6"/>
-    <mergeCell ref="AQ6:AT6"/>
-    <mergeCell ref="AU6:AX6"/>
-    <mergeCell ref="AY6:BB6"/>
+    <mergeCell ref="CM6:CP6"/>
     <mergeCell ref="AM7:AP7"/>
     <mergeCell ref="AQ7:AT7"/>
     <mergeCell ref="AU7:AX7"/>
@@ -4021,12 +4147,13 @@
     <mergeCell ref="AA7:AD7"/>
     <mergeCell ref="AE7:AH7"/>
     <mergeCell ref="AI7:AL7"/>
+    <mergeCell ref="DS7:DV7"/>
     <mergeCell ref="GU5:HF5"/>
     <mergeCell ref="HG5:HR5"/>
     <mergeCell ref="GI7:GL7"/>
     <mergeCell ref="GM7:GP7"/>
     <mergeCell ref="GQ7:GT7"/>
-    <mergeCell ref="HW7:HX7"/>
+    <mergeCell ref="IC7:ID7"/>
     <mergeCell ref="BK7:BN7"/>
     <mergeCell ref="BO7:BP7"/>
     <mergeCell ref="FO7:FR7"/>
@@ -4044,12 +4171,7 @@
     <mergeCell ref="CA6:CD6"/>
     <mergeCell ref="CE6:CH6"/>
     <mergeCell ref="CI6:CL6"/>
-    <mergeCell ref="CM6:CP6"/>
-    <mergeCell ref="CQ6:CT6"/>
-    <mergeCell ref="EI6:EL6"/>
-    <mergeCell ref="EM6:EP6"/>
-    <mergeCell ref="EQ6:ET6"/>
-    <mergeCell ref="EU6:EX6"/>
+    <mergeCell ref="DW7:DZ7"/>
     <mergeCell ref="EY6:FB6"/>
     <mergeCell ref="BS7:BV7"/>
     <mergeCell ref="BW7:BZ7"/>
@@ -4073,8 +4195,6 @@
     <mergeCell ref="DG7:DJ7"/>
     <mergeCell ref="DK7:DN7"/>
     <mergeCell ref="DO7:DR7"/>
-    <mergeCell ref="DS7:DV7"/>
-    <mergeCell ref="DW7:DZ7"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4087,7 +4207,7 @@
   <dimension ref="A2:HD14"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="U6" sqref="U6:V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4115,18 +4235,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:212" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
     </row>
     <row r="3" spans="1:212" s="14" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
@@ -4777,106 +4897,106 @@
     <row r="5" spans="1:212" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="103" t="s">
+      <c r="C5" s="106" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="104" t="s">
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="107" t="s">
         <v>130</v>
       </c>
-      <c r="L5" s="104"/>
-      <c r="M5" s="104"/>
-      <c r="N5" s="104"/>
-      <c r="O5" s="104"/>
-      <c r="P5" s="104"/>
-      <c r="Q5" s="104"/>
-      <c r="R5" s="104"/>
-      <c r="S5" s="104"/>
-      <c r="T5" s="104"/>
-      <c r="U5" s="104"/>
-      <c r="V5" s="104"/>
-      <c r="W5" s="105" t="s">
+      <c r="L5" s="107"/>
+      <c r="M5" s="107"/>
+      <c r="N5" s="107"/>
+      <c r="O5" s="107"/>
+      <c r="P5" s="107"/>
+      <c r="Q5" s="107"/>
+      <c r="R5" s="107"/>
+      <c r="S5" s="107"/>
+      <c r="T5" s="107"/>
+      <c r="U5" s="107"/>
+      <c r="V5" s="107"/>
+      <c r="W5" s="108" t="s">
         <v>146</v>
       </c>
-      <c r="X5" s="105"/>
-      <c r="Y5" s="105"/>
-      <c r="Z5" s="105"/>
-      <c r="AA5" s="105"/>
-      <c r="AB5" s="105"/>
-      <c r="AC5" s="105"/>
-      <c r="AD5" s="105"/>
-      <c r="AE5" s="105"/>
-      <c r="AF5" s="105"/>
-      <c r="AG5" s="105"/>
-      <c r="AH5" s="105"/>
-      <c r="AI5" s="105"/>
-      <c r="AJ5" s="105"/>
-      <c r="AK5" s="105"/>
-      <c r="AL5" s="105"/>
-      <c r="AM5" s="105"/>
-      <c r="AN5" s="105"/>
-      <c r="AO5" s="105"/>
-      <c r="AP5" s="105"/>
-      <c r="AQ5" s="105"/>
-      <c r="AR5" s="105"/>
-      <c r="AS5" s="105"/>
-      <c r="AT5" s="105"/>
-      <c r="AU5" s="105"/>
-      <c r="AV5" s="105"/>
-      <c r="AW5" s="105"/>
-      <c r="AX5" s="105"/>
-      <c r="AY5" s="105"/>
-      <c r="AZ5" s="105"/>
-      <c r="BA5" s="105"/>
-      <c r="BB5" s="105"/>
-      <c r="BC5" s="105"/>
-      <c r="BD5" s="105"/>
-      <c r="BE5" s="105"/>
-      <c r="BF5" s="105"/>
-      <c r="BG5" s="105"/>
-      <c r="BH5" s="105"/>
-      <c r="BI5" s="105"/>
-      <c r="BJ5" s="105"/>
-      <c r="BK5" s="105"/>
-      <c r="BL5" s="105"/>
-      <c r="BM5" s="105"/>
-      <c r="BN5" s="105"/>
-      <c r="BO5" s="105"/>
-      <c r="BP5" s="105"/>
-      <c r="BQ5" s="105"/>
-      <c r="BR5" s="105"/>
-      <c r="BS5" s="105"/>
-      <c r="BT5" s="105"/>
-      <c r="BU5" s="105"/>
-      <c r="BV5" s="105"/>
-      <c r="BW5" s="105"/>
-      <c r="BX5" s="105"/>
-      <c r="BY5" s="105"/>
-      <c r="BZ5" s="105"/>
-      <c r="CA5" s="106" t="s">
+      <c r="X5" s="108"/>
+      <c r="Y5" s="108"/>
+      <c r="Z5" s="108"/>
+      <c r="AA5" s="108"/>
+      <c r="AB5" s="108"/>
+      <c r="AC5" s="108"/>
+      <c r="AD5" s="108"/>
+      <c r="AE5" s="108"/>
+      <c r="AF5" s="108"/>
+      <c r="AG5" s="108"/>
+      <c r="AH5" s="108"/>
+      <c r="AI5" s="108"/>
+      <c r="AJ5" s="108"/>
+      <c r="AK5" s="108"/>
+      <c r="AL5" s="108"/>
+      <c r="AM5" s="108"/>
+      <c r="AN5" s="108"/>
+      <c r="AO5" s="108"/>
+      <c r="AP5" s="108"/>
+      <c r="AQ5" s="108"/>
+      <c r="AR5" s="108"/>
+      <c r="AS5" s="108"/>
+      <c r="AT5" s="108"/>
+      <c r="AU5" s="108"/>
+      <c r="AV5" s="108"/>
+      <c r="AW5" s="108"/>
+      <c r="AX5" s="108"/>
+      <c r="AY5" s="108"/>
+      <c r="AZ5" s="108"/>
+      <c r="BA5" s="108"/>
+      <c r="BB5" s="108"/>
+      <c r="BC5" s="108"/>
+      <c r="BD5" s="108"/>
+      <c r="BE5" s="108"/>
+      <c r="BF5" s="108"/>
+      <c r="BG5" s="108"/>
+      <c r="BH5" s="108"/>
+      <c r="BI5" s="108"/>
+      <c r="BJ5" s="108"/>
+      <c r="BK5" s="108"/>
+      <c r="BL5" s="108"/>
+      <c r="BM5" s="108"/>
+      <c r="BN5" s="108"/>
+      <c r="BO5" s="108"/>
+      <c r="BP5" s="108"/>
+      <c r="BQ5" s="108"/>
+      <c r="BR5" s="108"/>
+      <c r="BS5" s="108"/>
+      <c r="BT5" s="108"/>
+      <c r="BU5" s="108"/>
+      <c r="BV5" s="108"/>
+      <c r="BW5" s="108"/>
+      <c r="BX5" s="108"/>
+      <c r="BY5" s="108"/>
+      <c r="BZ5" s="108"/>
+      <c r="CA5" s="109" t="s">
         <v>158</v>
       </c>
-      <c r="CB5" s="107"/>
-      <c r="CC5" s="107"/>
-      <c r="CD5" s="107"/>
-      <c r="CE5" s="107"/>
-      <c r="CF5" s="107"/>
-      <c r="CG5" s="107"/>
-      <c r="CH5" s="107"/>
-      <c r="CI5" s="107"/>
-      <c r="CJ5" s="107"/>
-      <c r="CK5" s="107"/>
-      <c r="CL5" s="107"/>
-      <c r="CM5" s="107"/>
-      <c r="CN5" s="107"/>
-      <c r="CO5" s="107"/>
-      <c r="CP5" s="107"/>
+      <c r="CB5" s="110"/>
+      <c r="CC5" s="110"/>
+      <c r="CD5" s="110"/>
+      <c r="CE5" s="110"/>
+      <c r="CF5" s="110"/>
+      <c r="CG5" s="110"/>
+      <c r="CH5" s="110"/>
+      <c r="CI5" s="110"/>
+      <c r="CJ5" s="110"/>
+      <c r="CK5" s="110"/>
+      <c r="CL5" s="110"/>
+      <c r="CM5" s="110"/>
+      <c r="CN5" s="110"/>
+      <c r="CO5" s="110"/>
+      <c r="CP5" s="110"/>
       <c r="CQ5" s="66"/>
       <c r="CR5" s="66"/>
       <c r="CS5" s="66"/>
@@ -4943,210 +5063,210 @@
       <c r="EZ5" s="80"/>
       <c r="FA5" s="80"/>
       <c r="FB5" s="80"/>
-      <c r="FC5" s="81" t="s">
+      <c r="FC5" s="115" t="s">
         <v>209</v>
       </c>
-      <c r="FD5" s="82"/>
-      <c r="FE5" s="82"/>
-      <c r="FF5" s="82"/>
-      <c r="FG5" s="82"/>
-      <c r="FH5" s="82"/>
-      <c r="FI5" s="82"/>
-      <c r="FJ5" s="82"/>
-      <c r="FK5" s="82"/>
-      <c r="FL5" s="82"/>
-      <c r="FM5" s="82"/>
-      <c r="FN5" s="82"/>
-      <c r="FO5" s="82"/>
-      <c r="FP5" s="82"/>
-      <c r="FQ5" s="82"/>
-      <c r="FR5" s="82"/>
-      <c r="FS5" s="82"/>
-      <c r="FT5" s="82"/>
-      <c r="FU5" s="82"/>
-      <c r="FV5" s="82"/>
-      <c r="FW5" s="82"/>
-      <c r="FX5" s="82"/>
-      <c r="FY5" s="82"/>
-      <c r="FZ5" s="82"/>
-      <c r="GA5" s="82"/>
-      <c r="GB5" s="82"/>
-      <c r="GC5" s="82"/>
-      <c r="GD5" s="82"/>
-      <c r="GE5" s="82"/>
-      <c r="GF5" s="82"/>
-      <c r="GG5" s="82"/>
-      <c r="GH5" s="82"/>
-      <c r="GI5" s="82"/>
-      <c r="GJ5" s="82"/>
-      <c r="GK5" s="82"/>
-      <c r="GL5" s="82"/>
-      <c r="GM5" s="82"/>
-      <c r="GN5" s="82"/>
-      <c r="GO5" s="82"/>
-      <c r="GP5" s="82"/>
-      <c r="GQ5" s="82"/>
-      <c r="GR5" s="82"/>
-      <c r="GS5" s="82"/>
-      <c r="GT5" s="82"/>
-      <c r="GU5" s="82"/>
-      <c r="GV5" s="82"/>
-      <c r="GW5" s="82"/>
-      <c r="GX5" s="82"/>
+      <c r="FD5" s="116"/>
+      <c r="FE5" s="116"/>
+      <c r="FF5" s="116"/>
+      <c r="FG5" s="116"/>
+      <c r="FH5" s="116"/>
+      <c r="FI5" s="116"/>
+      <c r="FJ5" s="116"/>
+      <c r="FK5" s="116"/>
+      <c r="FL5" s="116"/>
+      <c r="FM5" s="116"/>
+      <c r="FN5" s="116"/>
+      <c r="FO5" s="116"/>
+      <c r="FP5" s="116"/>
+      <c r="FQ5" s="116"/>
+      <c r="FR5" s="116"/>
+      <c r="FS5" s="116"/>
+      <c r="FT5" s="116"/>
+      <c r="FU5" s="116"/>
+      <c r="FV5" s="116"/>
+      <c r="FW5" s="116"/>
+      <c r="FX5" s="116"/>
+      <c r="FY5" s="116"/>
+      <c r="FZ5" s="116"/>
+      <c r="GA5" s="116"/>
+      <c r="GB5" s="116"/>
+      <c r="GC5" s="116"/>
+      <c r="GD5" s="116"/>
+      <c r="GE5" s="116"/>
+      <c r="GF5" s="116"/>
+      <c r="GG5" s="116"/>
+      <c r="GH5" s="116"/>
+      <c r="GI5" s="116"/>
+      <c r="GJ5" s="116"/>
+      <c r="GK5" s="116"/>
+      <c r="GL5" s="116"/>
+      <c r="GM5" s="116"/>
+      <c r="GN5" s="116"/>
+      <c r="GO5" s="116"/>
+      <c r="GP5" s="116"/>
+      <c r="GQ5" s="116"/>
+      <c r="GR5" s="116"/>
+      <c r="GS5" s="116"/>
+      <c r="GT5" s="116"/>
+      <c r="GU5" s="116"/>
+      <c r="GV5" s="116"/>
+      <c r="GW5" s="116"/>
+      <c r="GX5" s="116"/>
       <c r="GY5" s="34"/>
       <c r="GZ5" s="34"/>
       <c r="HA5" s="34"/>
-      <c r="HB5" s="108" t="s">
+      <c r="HB5" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="HC5" s="109"/>
-      <c r="HD5" s="110"/>
+      <c r="HC5" s="113"/>
+      <c r="HD5" s="114"/>
     </row>
     <row r="6" spans="1:212" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="96" t="s">
+      <c r="C6" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="97"/>
-      <c r="E6" s="98"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="96"/>
       <c r="F6" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="G6" s="74" t="s">
+      <c r="G6" s="76" t="s">
         <v>122</v>
       </c>
-      <c r="H6" s="76"/>
-      <c r="I6" s="74" t="s">
+      <c r="H6" s="78"/>
+      <c r="I6" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="J6" s="76"/>
-      <c r="K6" s="99" t="s">
+      <c r="J6" s="78"/>
+      <c r="K6" s="97" t="s">
         <v>124</v>
       </c>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="101"/>
-      <c r="O6" s="99" t="s">
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="99"/>
+      <c r="O6" s="97" t="s">
         <v>125</v>
       </c>
-      <c r="P6" s="100"/>
-      <c r="Q6" s="100"/>
-      <c r="R6" s="101"/>
-      <c r="S6" s="99" t="s">
+      <c r="P6" s="98"/>
+      <c r="Q6" s="98"/>
+      <c r="R6" s="99"/>
+      <c r="S6" s="97" t="s">
         <v>126</v>
       </c>
-      <c r="T6" s="101"/>
-      <c r="U6" s="99" t="s">
+      <c r="T6" s="99"/>
+      <c r="U6" s="97" t="s">
         <v>127</v>
       </c>
-      <c r="V6" s="101"/>
-      <c r="W6" s="74" t="s">
+      <c r="V6" s="99"/>
+      <c r="W6" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="X6" s="76"/>
-      <c r="Y6" s="74" t="s">
+      <c r="X6" s="78"/>
+      <c r="Y6" s="76" t="s">
         <v>132</v>
       </c>
-      <c r="Z6" s="76"/>
-      <c r="AA6" s="74" t="s">
+      <c r="Z6" s="78"/>
+      <c r="AA6" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="AB6" s="75"/>
-      <c r="AC6" s="75"/>
-      <c r="AD6" s="76"/>
-      <c r="AE6" s="74" t="s">
+      <c r="AB6" s="77"/>
+      <c r="AC6" s="77"/>
+      <c r="AD6" s="78"/>
+      <c r="AE6" s="76" t="s">
         <v>134</v>
       </c>
-      <c r="AF6" s="75"/>
-      <c r="AG6" s="75"/>
-      <c r="AH6" s="76"/>
-      <c r="AI6" s="74" t="s">
+      <c r="AF6" s="77"/>
+      <c r="AG6" s="77"/>
+      <c r="AH6" s="78"/>
+      <c r="AI6" s="76" t="s">
         <v>135</v>
       </c>
-      <c r="AJ6" s="75"/>
-      <c r="AK6" s="75"/>
-      <c r="AL6" s="76"/>
-      <c r="AM6" s="74" t="s">
+      <c r="AJ6" s="77"/>
+      <c r="AK6" s="77"/>
+      <c r="AL6" s="78"/>
+      <c r="AM6" s="76" t="s">
         <v>136</v>
       </c>
-      <c r="AN6" s="75"/>
-      <c r="AO6" s="75"/>
-      <c r="AP6" s="76"/>
-      <c r="AQ6" s="74" t="s">
+      <c r="AN6" s="77"/>
+      <c r="AO6" s="77"/>
+      <c r="AP6" s="78"/>
+      <c r="AQ6" s="76" t="s">
         <v>137</v>
       </c>
-      <c r="AR6" s="75"/>
-      <c r="AS6" s="75"/>
-      <c r="AT6" s="76"/>
-      <c r="AU6" s="74" t="s">
+      <c r="AR6" s="77"/>
+      <c r="AS6" s="77"/>
+      <c r="AT6" s="78"/>
+      <c r="AU6" s="76" t="s">
         <v>138</v>
       </c>
-      <c r="AV6" s="75"/>
-      <c r="AW6" s="75"/>
-      <c r="AX6" s="76"/>
-      <c r="AY6" s="74" t="s">
+      <c r="AV6" s="77"/>
+      <c r="AW6" s="77"/>
+      <c r="AX6" s="78"/>
+      <c r="AY6" s="76" t="s">
         <v>139</v>
       </c>
-      <c r="AZ6" s="75"/>
-      <c r="BA6" s="75"/>
-      <c r="BB6" s="76"/>
-      <c r="BC6" s="74" t="s">
+      <c r="AZ6" s="77"/>
+      <c r="BA6" s="77"/>
+      <c r="BB6" s="78"/>
+      <c r="BC6" s="76" t="s">
         <v>140</v>
       </c>
-      <c r="BD6" s="75"/>
-      <c r="BE6" s="75"/>
-      <c r="BF6" s="76"/>
-      <c r="BG6" s="74" t="s">
+      <c r="BD6" s="77"/>
+      <c r="BE6" s="77"/>
+      <c r="BF6" s="78"/>
+      <c r="BG6" s="76" t="s">
         <v>141</v>
       </c>
-      <c r="BH6" s="75"/>
-      <c r="BI6" s="75"/>
-      <c r="BJ6" s="76"/>
-      <c r="BK6" s="74" t="s">
+      <c r="BH6" s="77"/>
+      <c r="BI6" s="77"/>
+      <c r="BJ6" s="78"/>
+      <c r="BK6" s="76" t="s">
         <v>142</v>
       </c>
-      <c r="BL6" s="75"/>
-      <c r="BM6" s="75"/>
-      <c r="BN6" s="76"/>
-      <c r="BO6" s="74" t="s">
+      <c r="BL6" s="77"/>
+      <c r="BM6" s="77"/>
+      <c r="BN6" s="78"/>
+      <c r="BO6" s="76" t="s">
         <v>143</v>
       </c>
-      <c r="BP6" s="75"/>
-      <c r="BQ6" s="75"/>
-      <c r="BR6" s="76"/>
-      <c r="BS6" s="74" t="s">
+      <c r="BP6" s="77"/>
+      <c r="BQ6" s="77"/>
+      <c r="BR6" s="78"/>
+      <c r="BS6" s="76" t="s">
         <v>144</v>
       </c>
-      <c r="BT6" s="75"/>
-      <c r="BU6" s="75"/>
-      <c r="BV6" s="76"/>
-      <c r="BW6" s="74" t="s">
+      <c r="BT6" s="77"/>
+      <c r="BU6" s="77"/>
+      <c r="BV6" s="78"/>
+      <c r="BW6" s="76" t="s">
         <v>145</v>
       </c>
-      <c r="BX6" s="76"/>
-      <c r="BY6" s="74" t="s">
+      <c r="BX6" s="78"/>
+      <c r="BY6" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="BZ6" s="76"/>
-      <c r="CA6" s="86" t="s">
+      <c r="BZ6" s="78"/>
+      <c r="CA6" s="100" t="s">
         <v>149</v>
       </c>
-      <c r="CB6" s="90"/>
-      <c r="CC6" s="90"/>
-      <c r="CD6" s="87"/>
-      <c r="CE6" s="86" t="s">
+      <c r="CB6" s="104"/>
+      <c r="CC6" s="104"/>
+      <c r="CD6" s="101"/>
+      <c r="CE6" s="100" t="s">
         <v>150</v>
       </c>
-      <c r="CF6" s="90"/>
-      <c r="CG6" s="90"/>
-      <c r="CH6" s="87"/>
-      <c r="CI6" s="86" t="s">
+      <c r="CF6" s="104"/>
+      <c r="CG6" s="104"/>
+      <c r="CH6" s="101"/>
+      <c r="CI6" s="100" t="s">
         <v>151</v>
       </c>
-      <c r="CJ6" s="87"/>
+      <c r="CJ6" s="101"/>
       <c r="CK6" s="40" t="s">
         <v>152</v>
       </c>
@@ -5165,30 +5285,30 @@
       <c r="CP6" s="40" t="s">
         <v>219</v>
       </c>
-      <c r="CQ6" s="74" t="s">
+      <c r="CQ6" s="76" t="s">
         <v>212</v>
       </c>
-      <c r="CR6" s="75"/>
-      <c r="CS6" s="75"/>
-      <c r="CT6" s="76"/>
-      <c r="CU6" s="74" t="s">
+      <c r="CR6" s="77"/>
+      <c r="CS6" s="77"/>
+      <c r="CT6" s="78"/>
+      <c r="CU6" s="76" t="s">
         <v>213</v>
       </c>
-      <c r="CV6" s="75"/>
-      <c r="CW6" s="75"/>
-      <c r="CX6" s="76"/>
-      <c r="CY6" s="74" t="s">
+      <c r="CV6" s="77"/>
+      <c r="CW6" s="77"/>
+      <c r="CX6" s="78"/>
+      <c r="CY6" s="76" t="s">
         <v>214</v>
       </c>
-      <c r="CZ6" s="75"/>
-      <c r="DA6" s="75"/>
-      <c r="DB6" s="76"/>
-      <c r="DC6" s="74" t="s">
+      <c r="CZ6" s="77"/>
+      <c r="DA6" s="77"/>
+      <c r="DB6" s="78"/>
+      <c r="DC6" s="76" t="s">
         <v>215</v>
       </c>
-      <c r="DD6" s="75"/>
-      <c r="DE6" s="75"/>
-      <c r="DF6" s="76"/>
+      <c r="DD6" s="77"/>
+      <c r="DE6" s="77"/>
+      <c r="DF6" s="78"/>
       <c r="DG6" s="42" t="s">
         <v>159</v>
       </c>
@@ -5489,14 +5609,14 @@
       <c r="HB6" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="HC6" s="88" t="s">
+      <c r="HC6" s="102" t="s">
         <v>210</v>
       </c>
-      <c r="HD6" s="89"/>
+      <c r="HD6" s="103"/>
     </row>
     <row r="7" spans="1:212" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="95"/>
+      <c r="B7" s="93"/>
       <c r="C7" s="20" t="s">
         <v>117</v>
       </c>
@@ -5509,142 +5629,142 @@
       <c r="F7" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="G7" s="72" t="s">
+      <c r="G7" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="H7" s="73"/>
+      <c r="H7" s="83"/>
       <c r="I7" s="2" t="s">
         <v>72</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="L7" s="70"/>
-      <c r="M7" s="70"/>
-      <c r="N7" s="71"/>
-      <c r="O7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="P7" s="70"/>
-      <c r="Q7" s="70"/>
-      <c r="R7" s="71"/>
-      <c r="S7" s="72" t="s">
+      <c r="K7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="75"/>
+      <c r="S7" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="T7" s="73"/>
-      <c r="U7" s="72" t="s">
+      <c r="T7" s="83"/>
+      <c r="U7" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="V7" s="73"/>
-      <c r="W7" s="72" t="s">
+      <c r="V7" s="83"/>
+      <c r="W7" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="X7" s="73"/>
-      <c r="Y7" s="72" t="s">
+      <c r="X7" s="83"/>
+      <c r="Y7" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="Z7" s="73"/>
-      <c r="AA7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB7" s="70"/>
-      <c r="AC7" s="70"/>
-      <c r="AD7" s="71"/>
-      <c r="AE7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="AF7" s="70"/>
-      <c r="AG7" s="70"/>
-      <c r="AH7" s="71"/>
-      <c r="AI7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="AJ7" s="70"/>
-      <c r="AK7" s="70"/>
-      <c r="AL7" s="71"/>
-      <c r="AM7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="AN7" s="70"/>
-      <c r="AO7" s="70"/>
-      <c r="AP7" s="71"/>
-      <c r="AQ7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="AR7" s="70"/>
-      <c r="AS7" s="70"/>
-      <c r="AT7" s="71"/>
-      <c r="AU7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="AV7" s="70"/>
-      <c r="AW7" s="70"/>
-      <c r="AX7" s="71"/>
-      <c r="AY7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="AZ7" s="70"/>
-      <c r="BA7" s="70"/>
-      <c r="BB7" s="71"/>
-      <c r="BC7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="BD7" s="70"/>
-      <c r="BE7" s="70"/>
-      <c r="BF7" s="71"/>
-      <c r="BG7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="BH7" s="70"/>
-      <c r="BI7" s="70"/>
-      <c r="BJ7" s="71"/>
-      <c r="BK7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="BL7" s="70"/>
-      <c r="BM7" s="70"/>
-      <c r="BN7" s="71"/>
-      <c r="BO7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="BP7" s="70"/>
-      <c r="BQ7" s="70"/>
-      <c r="BR7" s="71"/>
-      <c r="BS7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="BT7" s="70"/>
-      <c r="BU7" s="70"/>
-      <c r="BV7" s="71"/>
-      <c r="BW7" s="72" t="s">
+      <c r="Z7" s="83"/>
+      <c r="AA7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB7" s="74"/>
+      <c r="AC7" s="74"/>
+      <c r="AD7" s="75"/>
+      <c r="AE7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF7" s="74"/>
+      <c r="AG7" s="74"/>
+      <c r="AH7" s="75"/>
+      <c r="AI7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="AJ7" s="74"/>
+      <c r="AK7" s="74"/>
+      <c r="AL7" s="75"/>
+      <c r="AM7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="AN7" s="74"/>
+      <c r="AO7" s="74"/>
+      <c r="AP7" s="75"/>
+      <c r="AQ7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="AR7" s="74"/>
+      <c r="AS7" s="74"/>
+      <c r="AT7" s="75"/>
+      <c r="AU7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="AV7" s="74"/>
+      <c r="AW7" s="74"/>
+      <c r="AX7" s="75"/>
+      <c r="AY7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="AZ7" s="74"/>
+      <c r="BA7" s="74"/>
+      <c r="BB7" s="75"/>
+      <c r="BC7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="BD7" s="74"/>
+      <c r="BE7" s="74"/>
+      <c r="BF7" s="75"/>
+      <c r="BG7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="BH7" s="74"/>
+      <c r="BI7" s="74"/>
+      <c r="BJ7" s="75"/>
+      <c r="BK7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="BL7" s="74"/>
+      <c r="BM7" s="74"/>
+      <c r="BN7" s="75"/>
+      <c r="BO7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="BP7" s="74"/>
+      <c r="BQ7" s="74"/>
+      <c r="BR7" s="75"/>
+      <c r="BS7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="BT7" s="74"/>
+      <c r="BU7" s="74"/>
+      <c r="BV7" s="75"/>
+      <c r="BW7" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="BX7" s="73"/>
+      <c r="BX7" s="83"/>
       <c r="BY7" s="36" t="s">
         <v>72</v>
       </c>
       <c r="BZ7" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="CA7" s="83" t="s">
+      <c r="CA7" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="CB7" s="84"/>
-      <c r="CC7" s="84"/>
-      <c r="CD7" s="85"/>
-      <c r="CE7" s="83" t="s">
+      <c r="CB7" s="85"/>
+      <c r="CC7" s="85"/>
+      <c r="CD7" s="86"/>
+      <c r="CE7" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="CF7" s="84"/>
-      <c r="CG7" s="84"/>
-      <c r="CH7" s="85"/>
-      <c r="CI7" s="72" t="s">
+      <c r="CF7" s="85"/>
+      <c r="CG7" s="85"/>
+      <c r="CH7" s="86"/>
+      <c r="CI7" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="CJ7" s="73"/>
+      <c r="CJ7" s="83"/>
       <c r="CK7" s="35" t="s">
         <v>128</v>
       </c>
@@ -5663,30 +5783,30 @@
       <c r="CP7" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="CQ7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CR7" s="70"/>
-      <c r="CS7" s="70"/>
-      <c r="CT7" s="71"/>
-      <c r="CU7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CV7" s="70"/>
-      <c r="CW7" s="70"/>
-      <c r="CX7" s="71"/>
-      <c r="CY7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CZ7" s="70"/>
-      <c r="DA7" s="70"/>
-      <c r="DB7" s="71"/>
-      <c r="DC7" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DD7" s="70"/>
-      <c r="DE7" s="70"/>
-      <c r="DF7" s="71"/>
+      <c r="CQ7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CR7" s="74"/>
+      <c r="CS7" s="74"/>
+      <c r="CT7" s="75"/>
+      <c r="CU7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CV7" s="74"/>
+      <c r="CW7" s="74"/>
+      <c r="CX7" s="75"/>
+      <c r="CY7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CZ7" s="74"/>
+      <c r="DA7" s="74"/>
+      <c r="DB7" s="75"/>
+      <c r="DC7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DD7" s="74"/>
+      <c r="DE7" s="74"/>
+      <c r="DF7" s="75"/>
       <c r="DG7" s="35" t="s">
         <v>208</v>
       </c>
@@ -5987,10 +6107,10 @@
       <c r="HB7" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="HC7" s="72" t="s">
+      <c r="HC7" s="82" t="s">
         <v>211</v>
       </c>
-      <c r="HD7" s="73"/>
+      <c r="HD7" s="83"/>
     </row>
     <row r="8" spans="1:212" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -6017,138 +6137,138 @@
       <c r="CP9" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="CQ9" s="74" t="s">
+      <c r="CQ9" s="76" t="s">
         <v>220</v>
       </c>
-      <c r="CR9" s="75"/>
-      <c r="CS9" s="75"/>
-      <c r="CT9" s="76"/>
-      <c r="CU9" s="74" t="s">
+      <c r="CR9" s="77"/>
+      <c r="CS9" s="77"/>
+      <c r="CT9" s="78"/>
+      <c r="CU9" s="76" t="s">
         <v>221</v>
       </c>
-      <c r="CV9" s="75"/>
-      <c r="CW9" s="75"/>
-      <c r="CX9" s="76"/>
-      <c r="CY9" s="74" t="s">
+      <c r="CV9" s="77"/>
+      <c r="CW9" s="77"/>
+      <c r="CX9" s="78"/>
+      <c r="CY9" s="76" t="s">
         <v>222</v>
       </c>
-      <c r="CZ9" s="75"/>
-      <c r="DA9" s="75"/>
-      <c r="DB9" s="76"/>
-      <c r="DC9" s="74" t="s">
+      <c r="CZ9" s="77"/>
+      <c r="DA9" s="77"/>
+      <c r="DB9" s="78"/>
+      <c r="DC9" s="76" t="s">
         <v>223</v>
       </c>
-      <c r="DD9" s="75"/>
-      <c r="DE9" s="75"/>
-      <c r="DF9" s="76"/>
-      <c r="DG9" s="74" t="s">
+      <c r="DD9" s="77"/>
+      <c r="DE9" s="77"/>
+      <c r="DF9" s="78"/>
+      <c r="DG9" s="76" t="s">
         <v>224</v>
       </c>
-      <c r="DH9" s="75"/>
-      <c r="DI9" s="75"/>
-      <c r="DJ9" s="76"/>
-      <c r="DK9" s="74" t="s">
+      <c r="DH9" s="77"/>
+      <c r="DI9" s="77"/>
+      <c r="DJ9" s="78"/>
+      <c r="DK9" s="76" t="s">
         <v>225</v>
       </c>
-      <c r="DL9" s="75"/>
-      <c r="DM9" s="75"/>
-      <c r="DN9" s="76"/>
-      <c r="DO9" s="74" t="s">
+      <c r="DL9" s="77"/>
+      <c r="DM9" s="77"/>
+      <c r="DN9" s="78"/>
+      <c r="DO9" s="76" t="s">
         <v>226</v>
       </c>
-      <c r="DP9" s="75"/>
-      <c r="DQ9" s="75"/>
-      <c r="DR9" s="76"/>
-      <c r="DS9" s="74" t="s">
+      <c r="DP9" s="77"/>
+      <c r="DQ9" s="77"/>
+      <c r="DR9" s="78"/>
+      <c r="DS9" s="76" t="s">
         <v>227</v>
       </c>
-      <c r="DT9" s="75"/>
-      <c r="DU9" s="75"/>
-      <c r="DV9" s="76"/>
-      <c r="DW9" s="74" t="s">
+      <c r="DT9" s="77"/>
+      <c r="DU9" s="77"/>
+      <c r="DV9" s="78"/>
+      <c r="DW9" s="76" t="s">
         <v>228</v>
       </c>
-      <c r="DX9" s="75"/>
-      <c r="DY9" s="75"/>
-      <c r="DZ9" s="76"/>
-      <c r="EA9" s="74" t="s">
+      <c r="DX9" s="77"/>
+      <c r="DY9" s="77"/>
+      <c r="DZ9" s="78"/>
+      <c r="EA9" s="76" t="s">
         <v>229</v>
       </c>
-      <c r="EB9" s="75"/>
-      <c r="EC9" s="75"/>
-      <c r="ED9" s="76"/>
-      <c r="EE9" s="74" t="s">
+      <c r="EB9" s="77"/>
+      <c r="EC9" s="77"/>
+      <c r="ED9" s="78"/>
+      <c r="EE9" s="76" t="s">
         <v>230</v>
       </c>
-      <c r="EF9" s="75"/>
-      <c r="EG9" s="75"/>
-      <c r="EH9" s="76"/>
-      <c r="EI9" s="74" t="s">
+      <c r="EF9" s="77"/>
+      <c r="EG9" s="77"/>
+      <c r="EH9" s="78"/>
+      <c r="EI9" s="76" t="s">
         <v>220</v>
       </c>
-      <c r="EJ9" s="75"/>
-      <c r="EK9" s="75"/>
-      <c r="EL9" s="76"/>
-      <c r="EM9" s="74" t="s">
+      <c r="EJ9" s="77"/>
+      <c r="EK9" s="77"/>
+      <c r="EL9" s="78"/>
+      <c r="EM9" s="76" t="s">
         <v>221</v>
       </c>
-      <c r="EN9" s="75"/>
-      <c r="EO9" s="75"/>
-      <c r="EP9" s="76"/>
-      <c r="EQ9" s="74" t="s">
+      <c r="EN9" s="77"/>
+      <c r="EO9" s="77"/>
+      <c r="EP9" s="78"/>
+      <c r="EQ9" s="76" t="s">
         <v>222</v>
       </c>
-      <c r="ER9" s="75"/>
-      <c r="ES9" s="75"/>
-      <c r="ET9" s="76"/>
-      <c r="EU9" s="74" t="s">
+      <c r="ER9" s="77"/>
+      <c r="ES9" s="77"/>
+      <c r="ET9" s="78"/>
+      <c r="EU9" s="76" t="s">
         <v>223</v>
       </c>
-      <c r="EV9" s="75"/>
-      <c r="EW9" s="75"/>
-      <c r="EX9" s="76"/>
-      <c r="EY9" s="74" t="s">
+      <c r="EV9" s="77"/>
+      <c r="EW9" s="77"/>
+      <c r="EX9" s="78"/>
+      <c r="EY9" s="76" t="s">
         <v>224</v>
       </c>
-      <c r="EZ9" s="75"/>
-      <c r="FA9" s="75"/>
-      <c r="FB9" s="76"/>
-      <c r="FC9" s="74" t="s">
+      <c r="EZ9" s="77"/>
+      <c r="FA9" s="77"/>
+      <c r="FB9" s="78"/>
+      <c r="FC9" s="76" t="s">
         <v>225</v>
       </c>
-      <c r="FD9" s="75"/>
-      <c r="FE9" s="75"/>
-      <c r="FF9" s="76"/>
-      <c r="FG9" s="74" t="s">
+      <c r="FD9" s="77"/>
+      <c r="FE9" s="77"/>
+      <c r="FF9" s="78"/>
+      <c r="FG9" s="76" t="s">
         <v>226</v>
       </c>
-      <c r="FH9" s="75"/>
-      <c r="FI9" s="75"/>
-      <c r="FJ9" s="76"/>
-      <c r="FK9" s="74" t="s">
+      <c r="FH9" s="77"/>
+      <c r="FI9" s="77"/>
+      <c r="FJ9" s="78"/>
+      <c r="FK9" s="76" t="s">
         <v>227</v>
       </c>
-      <c r="FL9" s="75"/>
-      <c r="FM9" s="75"/>
-      <c r="FN9" s="76"/>
-      <c r="FO9" s="74" t="s">
+      <c r="FL9" s="77"/>
+      <c r="FM9" s="77"/>
+      <c r="FN9" s="78"/>
+      <c r="FO9" s="76" t="s">
         <v>228</v>
       </c>
-      <c r="FP9" s="75"/>
-      <c r="FQ9" s="75"/>
-      <c r="FR9" s="76"/>
-      <c r="FS9" s="74" t="s">
+      <c r="FP9" s="77"/>
+      <c r="FQ9" s="77"/>
+      <c r="FR9" s="78"/>
+      <c r="FS9" s="76" t="s">
         <v>229</v>
       </c>
-      <c r="FT9" s="75"/>
-      <c r="FU9" s="75"/>
-      <c r="FV9" s="76"/>
-      <c r="FW9" s="74" t="s">
+      <c r="FT9" s="77"/>
+      <c r="FU9" s="77"/>
+      <c r="FV9" s="78"/>
+      <c r="FW9" s="76" t="s">
         <v>230</v>
       </c>
-      <c r="FX9" s="75"/>
-      <c r="FY9" s="75"/>
-      <c r="FZ9" s="76"/>
+      <c r="FX9" s="77"/>
+      <c r="FY9" s="77"/>
+      <c r="FZ9" s="78"/>
     </row>
     <row r="10" spans="1:212" x14ac:dyDescent="0.25">
       <c r="CM10" s="39" t="s">
@@ -6163,138 +6283,138 @@
       <c r="CP10" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="CQ10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CR10" s="70"/>
-      <c r="CS10" s="70"/>
-      <c r="CT10" s="71"/>
-      <c r="CU10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CV10" s="70"/>
-      <c r="CW10" s="70"/>
-      <c r="CX10" s="71"/>
-      <c r="CY10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CZ10" s="70"/>
-      <c r="DA10" s="70"/>
-      <c r="DB10" s="71"/>
-      <c r="DC10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DD10" s="70"/>
-      <c r="DE10" s="70"/>
-      <c r="DF10" s="71"/>
-      <c r="DG10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DH10" s="70"/>
-      <c r="DI10" s="70"/>
-      <c r="DJ10" s="71"/>
-      <c r="DK10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DL10" s="70"/>
-      <c r="DM10" s="70"/>
-      <c r="DN10" s="71"/>
-      <c r="DO10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DP10" s="70"/>
-      <c r="DQ10" s="70"/>
-      <c r="DR10" s="71"/>
-      <c r="DS10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT10" s="70"/>
-      <c r="DU10" s="70"/>
-      <c r="DV10" s="71"/>
-      <c r="DW10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DX10" s="70"/>
-      <c r="DY10" s="70"/>
-      <c r="DZ10" s="71"/>
-      <c r="EA10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EB10" s="70"/>
-      <c r="EC10" s="70"/>
-      <c r="ED10" s="71"/>
-      <c r="EE10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EF10" s="70"/>
-      <c r="EG10" s="70"/>
-      <c r="EH10" s="71"/>
-      <c r="EI10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EJ10" s="70"/>
-      <c r="EK10" s="70"/>
-      <c r="EL10" s="71"/>
-      <c r="EM10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EN10" s="70"/>
-      <c r="EO10" s="70"/>
-      <c r="EP10" s="71"/>
-      <c r="EQ10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="ER10" s="70"/>
-      <c r="ES10" s="70"/>
-      <c r="ET10" s="71"/>
-      <c r="EU10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EV10" s="70"/>
-      <c r="EW10" s="70"/>
-      <c r="EX10" s="71"/>
-      <c r="EY10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EZ10" s="70"/>
-      <c r="FA10" s="70"/>
-      <c r="FB10" s="71"/>
-      <c r="FC10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="FD10" s="70"/>
-      <c r="FE10" s="70"/>
-      <c r="FF10" s="71"/>
-      <c r="FG10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="FH10" s="70"/>
-      <c r="FI10" s="70"/>
-      <c r="FJ10" s="71"/>
-      <c r="FK10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="FL10" s="70"/>
-      <c r="FM10" s="70"/>
-      <c r="FN10" s="71"/>
-      <c r="FO10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="FP10" s="70"/>
-      <c r="FQ10" s="70"/>
-      <c r="FR10" s="71"/>
-      <c r="FS10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="FT10" s="70"/>
-      <c r="FU10" s="70"/>
-      <c r="FV10" s="71"/>
-      <c r="FW10" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="FX10" s="70"/>
-      <c r="FY10" s="70"/>
-      <c r="FZ10" s="71"/>
+      <c r="CQ10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CR10" s="74"/>
+      <c r="CS10" s="74"/>
+      <c r="CT10" s="75"/>
+      <c r="CU10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CV10" s="74"/>
+      <c r="CW10" s="74"/>
+      <c r="CX10" s="75"/>
+      <c r="CY10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CZ10" s="74"/>
+      <c r="DA10" s="74"/>
+      <c r="DB10" s="75"/>
+      <c r="DC10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DD10" s="74"/>
+      <c r="DE10" s="74"/>
+      <c r="DF10" s="75"/>
+      <c r="DG10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DH10" s="74"/>
+      <c r="DI10" s="74"/>
+      <c r="DJ10" s="75"/>
+      <c r="DK10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL10" s="74"/>
+      <c r="DM10" s="74"/>
+      <c r="DN10" s="75"/>
+      <c r="DO10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DP10" s="74"/>
+      <c r="DQ10" s="74"/>
+      <c r="DR10" s="75"/>
+      <c r="DS10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DT10" s="74"/>
+      <c r="DU10" s="74"/>
+      <c r="DV10" s="75"/>
+      <c r="DW10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DX10" s="74"/>
+      <c r="DY10" s="74"/>
+      <c r="DZ10" s="75"/>
+      <c r="EA10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EB10" s="74"/>
+      <c r="EC10" s="74"/>
+      <c r="ED10" s="75"/>
+      <c r="EE10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EF10" s="74"/>
+      <c r="EG10" s="74"/>
+      <c r="EH10" s="75"/>
+      <c r="EI10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EJ10" s="74"/>
+      <c r="EK10" s="74"/>
+      <c r="EL10" s="75"/>
+      <c r="EM10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EN10" s="74"/>
+      <c r="EO10" s="74"/>
+      <c r="EP10" s="75"/>
+      <c r="EQ10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="ER10" s="74"/>
+      <c r="ES10" s="74"/>
+      <c r="ET10" s="75"/>
+      <c r="EU10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EV10" s="74"/>
+      <c r="EW10" s="74"/>
+      <c r="EX10" s="75"/>
+      <c r="EY10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EZ10" s="74"/>
+      <c r="FA10" s="74"/>
+      <c r="FB10" s="75"/>
+      <c r="FC10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="FD10" s="74"/>
+      <c r="FE10" s="74"/>
+      <c r="FF10" s="75"/>
+      <c r="FG10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="FH10" s="74"/>
+      <c r="FI10" s="74"/>
+      <c r="FJ10" s="75"/>
+      <c r="FK10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="FL10" s="74"/>
+      <c r="FM10" s="74"/>
+      <c r="FN10" s="75"/>
+      <c r="FO10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="FP10" s="74"/>
+      <c r="FQ10" s="74"/>
+      <c r="FR10" s="75"/>
+      <c r="FS10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="FT10" s="74"/>
+      <c r="FU10" s="74"/>
+      <c r="FV10" s="75"/>
+      <c r="FW10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="FX10" s="74"/>
+      <c r="FY10" s="74"/>
+      <c r="FZ10" s="75"/>
     </row>
     <row r="12" spans="1:212" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -6321,138 +6441,138 @@
       <c r="CP13" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="CQ13" s="74" t="s">
+      <c r="CQ13" s="76" t="s">
         <v>220</v>
       </c>
-      <c r="CR13" s="75"/>
-      <c r="CS13" s="75"/>
-      <c r="CT13" s="76"/>
-      <c r="CU13" s="74" t="s">
+      <c r="CR13" s="77"/>
+      <c r="CS13" s="77"/>
+      <c r="CT13" s="78"/>
+      <c r="CU13" s="76" t="s">
         <v>221</v>
       </c>
-      <c r="CV13" s="75"/>
-      <c r="CW13" s="75"/>
-      <c r="CX13" s="76"/>
-      <c r="CY13" s="74" t="s">
+      <c r="CV13" s="77"/>
+      <c r="CW13" s="77"/>
+      <c r="CX13" s="78"/>
+      <c r="CY13" s="76" t="s">
         <v>222</v>
       </c>
-      <c r="CZ13" s="75"/>
-      <c r="DA13" s="75"/>
-      <c r="DB13" s="76"/>
-      <c r="DC13" s="74" t="s">
+      <c r="CZ13" s="77"/>
+      <c r="DA13" s="77"/>
+      <c r="DB13" s="78"/>
+      <c r="DC13" s="76" t="s">
         <v>223</v>
       </c>
-      <c r="DD13" s="75"/>
-      <c r="DE13" s="75"/>
-      <c r="DF13" s="76"/>
-      <c r="DG13" s="74" t="s">
+      <c r="DD13" s="77"/>
+      <c r="DE13" s="77"/>
+      <c r="DF13" s="78"/>
+      <c r="DG13" s="76" t="s">
         <v>224</v>
       </c>
-      <c r="DH13" s="75"/>
-      <c r="DI13" s="75"/>
-      <c r="DJ13" s="76"/>
-      <c r="DK13" s="74" t="s">
+      <c r="DH13" s="77"/>
+      <c r="DI13" s="77"/>
+      <c r="DJ13" s="78"/>
+      <c r="DK13" s="76" t="s">
         <v>225</v>
       </c>
-      <c r="DL13" s="75"/>
-      <c r="DM13" s="75"/>
-      <c r="DN13" s="76"/>
-      <c r="DO13" s="74" t="s">
+      <c r="DL13" s="77"/>
+      <c r="DM13" s="77"/>
+      <c r="DN13" s="78"/>
+      <c r="DO13" s="76" t="s">
         <v>226</v>
       </c>
-      <c r="DP13" s="75"/>
-      <c r="DQ13" s="75"/>
-      <c r="DR13" s="76"/>
-      <c r="DS13" s="74" t="s">
+      <c r="DP13" s="77"/>
+      <c r="DQ13" s="77"/>
+      <c r="DR13" s="78"/>
+      <c r="DS13" s="76" t="s">
         <v>227</v>
       </c>
-      <c r="DT13" s="75"/>
-      <c r="DU13" s="75"/>
-      <c r="DV13" s="76"/>
-      <c r="DW13" s="74" t="s">
+      <c r="DT13" s="77"/>
+      <c r="DU13" s="77"/>
+      <c r="DV13" s="78"/>
+      <c r="DW13" s="76" t="s">
         <v>228</v>
       </c>
-      <c r="DX13" s="75"/>
-      <c r="DY13" s="75"/>
-      <c r="DZ13" s="76"/>
-      <c r="EA13" s="74" t="s">
+      <c r="DX13" s="77"/>
+      <c r="DY13" s="77"/>
+      <c r="DZ13" s="78"/>
+      <c r="EA13" s="76" t="s">
         <v>229</v>
       </c>
-      <c r="EB13" s="75"/>
-      <c r="EC13" s="75"/>
-      <c r="ED13" s="76"/>
-      <c r="EE13" s="74" t="s">
+      <c r="EB13" s="77"/>
+      <c r="EC13" s="77"/>
+      <c r="ED13" s="78"/>
+      <c r="EE13" s="76" t="s">
         <v>230</v>
       </c>
-      <c r="EF13" s="75"/>
-      <c r="EG13" s="75"/>
-      <c r="EH13" s="76"/>
-      <c r="EI13" s="74" t="s">
+      <c r="EF13" s="77"/>
+      <c r="EG13" s="77"/>
+      <c r="EH13" s="78"/>
+      <c r="EI13" s="76" t="s">
         <v>220</v>
       </c>
-      <c r="EJ13" s="75"/>
-      <c r="EK13" s="75"/>
-      <c r="EL13" s="76"/>
-      <c r="EM13" s="74" t="s">
+      <c r="EJ13" s="77"/>
+      <c r="EK13" s="77"/>
+      <c r="EL13" s="78"/>
+      <c r="EM13" s="76" t="s">
         <v>221</v>
       </c>
-      <c r="EN13" s="75"/>
-      <c r="EO13" s="75"/>
-      <c r="EP13" s="76"/>
-      <c r="EQ13" s="74" t="s">
+      <c r="EN13" s="77"/>
+      <c r="EO13" s="77"/>
+      <c r="EP13" s="78"/>
+      <c r="EQ13" s="76" t="s">
         <v>222</v>
       </c>
-      <c r="ER13" s="75"/>
-      <c r="ES13" s="75"/>
-      <c r="ET13" s="76"/>
-      <c r="EU13" s="74" t="s">
+      <c r="ER13" s="77"/>
+      <c r="ES13" s="77"/>
+      <c r="ET13" s="78"/>
+      <c r="EU13" s="76" t="s">
         <v>223</v>
       </c>
-      <c r="EV13" s="75"/>
-      <c r="EW13" s="75"/>
-      <c r="EX13" s="76"/>
-      <c r="EY13" s="74" t="s">
+      <c r="EV13" s="77"/>
+      <c r="EW13" s="77"/>
+      <c r="EX13" s="78"/>
+      <c r="EY13" s="76" t="s">
         <v>224</v>
       </c>
-      <c r="EZ13" s="75"/>
-      <c r="FA13" s="75"/>
-      <c r="FB13" s="76"/>
-      <c r="FC13" s="74" t="s">
+      <c r="EZ13" s="77"/>
+      <c r="FA13" s="77"/>
+      <c r="FB13" s="78"/>
+      <c r="FC13" s="76" t="s">
         <v>225</v>
       </c>
-      <c r="FD13" s="75"/>
-      <c r="FE13" s="75"/>
-      <c r="FF13" s="76"/>
-      <c r="FG13" s="74" t="s">
+      <c r="FD13" s="77"/>
+      <c r="FE13" s="77"/>
+      <c r="FF13" s="78"/>
+      <c r="FG13" s="76" t="s">
         <v>226</v>
       </c>
-      <c r="FH13" s="75"/>
-      <c r="FI13" s="75"/>
-      <c r="FJ13" s="76"/>
-      <c r="FK13" s="74" t="s">
+      <c r="FH13" s="77"/>
+      <c r="FI13" s="77"/>
+      <c r="FJ13" s="78"/>
+      <c r="FK13" s="76" t="s">
         <v>227</v>
       </c>
-      <c r="FL13" s="75"/>
-      <c r="FM13" s="75"/>
-      <c r="FN13" s="76"/>
-      <c r="FO13" s="74" t="s">
+      <c r="FL13" s="77"/>
+      <c r="FM13" s="77"/>
+      <c r="FN13" s="78"/>
+      <c r="FO13" s="76" t="s">
         <v>228</v>
       </c>
-      <c r="FP13" s="75"/>
-      <c r="FQ13" s="75"/>
-      <c r="FR13" s="76"/>
-      <c r="FS13" s="74" t="s">
+      <c r="FP13" s="77"/>
+      <c r="FQ13" s="77"/>
+      <c r="FR13" s="78"/>
+      <c r="FS13" s="76" t="s">
         <v>229</v>
       </c>
-      <c r="FT13" s="75"/>
-      <c r="FU13" s="75"/>
-      <c r="FV13" s="76"/>
-      <c r="FW13" s="74" t="s">
+      <c r="FT13" s="77"/>
+      <c r="FU13" s="77"/>
+      <c r="FV13" s="78"/>
+      <c r="FW13" s="76" t="s">
         <v>230</v>
       </c>
-      <c r="FX13" s="75"/>
-      <c r="FY13" s="75"/>
-      <c r="FZ13" s="76"/>
+      <c r="FX13" s="77"/>
+      <c r="FY13" s="77"/>
+      <c r="FZ13" s="78"/>
     </row>
     <row r="14" spans="1:212" x14ac:dyDescent="0.25">
       <c r="CM14" s="39" t="s">
@@ -6467,138 +6587,138 @@
       <c r="CP14" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="CQ14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CR14" s="70"/>
-      <c r="CS14" s="70"/>
-      <c r="CT14" s="71"/>
-      <c r="CU14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CV14" s="70"/>
-      <c r="CW14" s="70"/>
-      <c r="CX14" s="71"/>
-      <c r="CY14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="CZ14" s="70"/>
-      <c r="DA14" s="70"/>
-      <c r="DB14" s="71"/>
-      <c r="DC14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DD14" s="70"/>
-      <c r="DE14" s="70"/>
-      <c r="DF14" s="71"/>
-      <c r="DG14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DH14" s="70"/>
-      <c r="DI14" s="70"/>
-      <c r="DJ14" s="71"/>
-      <c r="DK14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DL14" s="70"/>
-      <c r="DM14" s="70"/>
-      <c r="DN14" s="71"/>
-      <c r="DO14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DP14" s="70"/>
-      <c r="DQ14" s="70"/>
-      <c r="DR14" s="71"/>
-      <c r="DS14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT14" s="70"/>
-      <c r="DU14" s="70"/>
-      <c r="DV14" s="71"/>
-      <c r="DW14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="DX14" s="70"/>
-      <c r="DY14" s="70"/>
-      <c r="DZ14" s="71"/>
-      <c r="EA14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EB14" s="70"/>
-      <c r="EC14" s="70"/>
-      <c r="ED14" s="71"/>
-      <c r="EE14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EF14" s="70"/>
-      <c r="EG14" s="70"/>
-      <c r="EH14" s="71"/>
-      <c r="EI14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EJ14" s="70"/>
-      <c r="EK14" s="70"/>
-      <c r="EL14" s="71"/>
-      <c r="EM14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EN14" s="70"/>
-      <c r="EO14" s="70"/>
-      <c r="EP14" s="71"/>
-      <c r="EQ14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="ER14" s="70"/>
-      <c r="ES14" s="70"/>
-      <c r="ET14" s="71"/>
-      <c r="EU14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EV14" s="70"/>
-      <c r="EW14" s="70"/>
-      <c r="EX14" s="71"/>
-      <c r="EY14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="EZ14" s="70"/>
-      <c r="FA14" s="70"/>
-      <c r="FB14" s="71"/>
-      <c r="FC14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="FD14" s="70"/>
-      <c r="FE14" s="70"/>
-      <c r="FF14" s="71"/>
-      <c r="FG14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="FH14" s="70"/>
-      <c r="FI14" s="70"/>
-      <c r="FJ14" s="71"/>
-      <c r="FK14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="FL14" s="70"/>
-      <c r="FM14" s="70"/>
-      <c r="FN14" s="71"/>
-      <c r="FO14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="FP14" s="70"/>
-      <c r="FQ14" s="70"/>
-      <c r="FR14" s="71"/>
-      <c r="FS14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="FT14" s="70"/>
-      <c r="FU14" s="70"/>
-      <c r="FV14" s="71"/>
-      <c r="FW14" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="FX14" s="70"/>
-      <c r="FY14" s="70"/>
-      <c r="FZ14" s="71"/>
+      <c r="CQ14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CR14" s="74"/>
+      <c r="CS14" s="74"/>
+      <c r="CT14" s="75"/>
+      <c r="CU14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CV14" s="74"/>
+      <c r="CW14" s="74"/>
+      <c r="CX14" s="75"/>
+      <c r="CY14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="CZ14" s="74"/>
+      <c r="DA14" s="74"/>
+      <c r="DB14" s="75"/>
+      <c r="DC14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DD14" s="74"/>
+      <c r="DE14" s="74"/>
+      <c r="DF14" s="75"/>
+      <c r="DG14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DH14" s="74"/>
+      <c r="DI14" s="74"/>
+      <c r="DJ14" s="75"/>
+      <c r="DK14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL14" s="74"/>
+      <c r="DM14" s="74"/>
+      <c r="DN14" s="75"/>
+      <c r="DO14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DP14" s="74"/>
+      <c r="DQ14" s="74"/>
+      <c r="DR14" s="75"/>
+      <c r="DS14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DT14" s="74"/>
+      <c r="DU14" s="74"/>
+      <c r="DV14" s="75"/>
+      <c r="DW14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="DX14" s="74"/>
+      <c r="DY14" s="74"/>
+      <c r="DZ14" s="75"/>
+      <c r="EA14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EB14" s="74"/>
+      <c r="EC14" s="74"/>
+      <c r="ED14" s="75"/>
+      <c r="EE14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EF14" s="74"/>
+      <c r="EG14" s="74"/>
+      <c r="EH14" s="75"/>
+      <c r="EI14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EJ14" s="74"/>
+      <c r="EK14" s="74"/>
+      <c r="EL14" s="75"/>
+      <c r="EM14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EN14" s="74"/>
+      <c r="EO14" s="74"/>
+      <c r="EP14" s="75"/>
+      <c r="EQ14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="ER14" s="74"/>
+      <c r="ES14" s="74"/>
+      <c r="ET14" s="75"/>
+      <c r="EU14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EV14" s="74"/>
+      <c r="EW14" s="74"/>
+      <c r="EX14" s="75"/>
+      <c r="EY14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="EZ14" s="74"/>
+      <c r="FA14" s="74"/>
+      <c r="FB14" s="75"/>
+      <c r="FC14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="FD14" s="74"/>
+      <c r="FE14" s="74"/>
+      <c r="FF14" s="75"/>
+      <c r="FG14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="FH14" s="74"/>
+      <c r="FI14" s="74"/>
+      <c r="FJ14" s="75"/>
+      <c r="FK14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="FL14" s="74"/>
+      <c r="FM14" s="74"/>
+      <c r="FN14" s="75"/>
+      <c r="FO14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="FP14" s="74"/>
+      <c r="FQ14" s="74"/>
+      <c r="FR14" s="75"/>
+      <c r="FS14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="FT14" s="74"/>
+      <c r="FU14" s="74"/>
+      <c r="FV14" s="75"/>
+      <c r="FW14" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="FX14" s="74"/>
+      <c r="FY14" s="74"/>
+      <c r="FZ14" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="156">
@@ -6657,7 +6777,6 @@
     <mergeCell ref="AA6:AD6"/>
     <mergeCell ref="AE6:AH6"/>
     <mergeCell ref="BC6:BF6"/>
-    <mergeCell ref="BG6:BJ6"/>
     <mergeCell ref="BK6:BN6"/>
     <mergeCell ref="AI6:AL6"/>
     <mergeCell ref="BO6:BR6"/>
@@ -6694,6 +6813,7 @@
     <mergeCell ref="CU7:CX7"/>
     <mergeCell ref="CY7:DB7"/>
     <mergeCell ref="DC7:DF7"/>
+    <mergeCell ref="BG6:BJ6"/>
     <mergeCell ref="FK13:FN13"/>
     <mergeCell ref="FO13:FR13"/>
     <mergeCell ref="FS13:FV13"/>
@@ -6783,49 +6903,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:52" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="131" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="125"/>
-      <c r="O2" s="125"/>
-      <c r="P2" s="125"/>
-      <c r="Q2" s="125"/>
-      <c r="R2" s="125"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="125"/>
-      <c r="U2" s="125"/>
-      <c r="V2" s="125"/>
-      <c r="W2" s="125"/>
-      <c r="X2" s="125"/>
-      <c r="Y2" s="125"/>
-      <c r="Z2" s="125"/>
-      <c r="AA2" s="125"/>
-      <c r="AB2" s="125"/>
-      <c r="AC2" s="125"/>
-      <c r="AD2" s="125"/>
-      <c r="AE2" s="125"/>
-      <c r="AF2" s="125"/>
-      <c r="AG2" s="125"/>
-      <c r="AH2" s="125"/>
-      <c r="AI2" s="125"/>
-      <c r="AJ2" s="125"/>
-      <c r="AK2" s="125"/>
-      <c r="AL2" s="125"/>
-      <c r="AM2" s="125"/>
-      <c r="AN2" s="125"/>
-      <c r="AO2" s="125"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="131"/>
+      <c r="P2" s="131"/>
+      <c r="Q2" s="131"/>
+      <c r="R2" s="131"/>
+      <c r="S2" s="131"/>
+      <c r="T2" s="131"/>
+      <c r="U2" s="131"/>
+      <c r="V2" s="131"/>
+      <c r="W2" s="131"/>
+      <c r="X2" s="131"/>
+      <c r="Y2" s="131"/>
+      <c r="Z2" s="131"/>
+      <c r="AA2" s="131"/>
+      <c r="AB2" s="131"/>
+      <c r="AC2" s="131"/>
+      <c r="AD2" s="131"/>
+      <c r="AE2" s="131"/>
+      <c r="AF2" s="131"/>
+      <c r="AG2" s="131"/>
+      <c r="AH2" s="131"/>
+      <c r="AI2" s="131"/>
+      <c r="AJ2" s="131"/>
+      <c r="AK2" s="131"/>
+      <c r="AL2" s="131"/>
+      <c r="AM2" s="131"/>
+      <c r="AN2" s="131"/>
+      <c r="AO2" s="131"/>
       <c r="AP2" s="31"/>
       <c r="AQ2" s="31"/>
       <c r="AR2" s="31"/>
@@ -7029,7 +7149,7 @@
       <c r="AZ4" s="29"/>
     </row>
     <row r="5" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="114" t="s">
+      <c r="B5" s="120" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="23" t="s">
@@ -7164,17 +7284,17 @@
       <c r="AT5" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="AU5" s="113" t="s">
+      <c r="AU5" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="AV5" s="113"/>
+      <c r="AV5" s="119"/>
       <c r="AW5" s="29"/>
       <c r="AX5" s="29"/>
       <c r="AY5" s="29"/>
       <c r="AZ5" s="29"/>
     </row>
     <row r="6" spans="1:52" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="115"/>
+      <c r="B6" s="121"/>
       <c r="C6" s="20" t="s">
         <v>87</v>
       </c>
@@ -7364,7 +7484,7 @@
       <c r="AV7" s="7"/>
     </row>
     <row r="8" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="114" t="s">
+      <c r="B8" s="120" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -7499,13 +7619,13 @@
       <c r="AT8" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="AU8" s="111" t="s">
+      <c r="AU8" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="AV8" s="112"/>
+      <c r="AV8" s="118"/>
     </row>
     <row r="9" spans="1:52" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="115"/>
+      <c r="B9" s="121"/>
       <c r="C9" s="20" t="s">
         <v>87</v>
       </c>
@@ -7691,7 +7811,7 @@
       <c r="AV10" s="7"/>
     </row>
     <row r="11" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="114" t="s">
+      <c r="B11" s="120" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -7826,13 +7946,13 @@
       <c r="AT11" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="AU11" s="111" t="s">
+      <c r="AU11" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="AV11" s="112"/>
+      <c r="AV11" s="118"/>
     </row>
     <row r="12" spans="1:52" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="115"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="20" t="s">
         <v>87</v>
       </c>
@@ -8018,7 +8138,7 @@
       <c r="AV13" s="7"/>
     </row>
     <row r="14" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="114" t="s">
+      <c r="B14" s="120" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -8153,13 +8273,13 @@
       <c r="AT14" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="AU14" s="111" t="s">
+      <c r="AU14" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="AV14" s="112"/>
+      <c r="AV14" s="118"/>
     </row>
     <row r="15" spans="1:52" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="115"/>
+      <c r="B15" s="121"/>
       <c r="C15" s="20" t="s">
         <v>87</v>
       </c>
@@ -8311,7 +8431,7 @@
       <c r="AV16" s="7"/>
     </row>
     <row r="17" spans="2:48" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="114" t="s">
+      <c r="B17" s="120" t="s">
         <v>71</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -8446,13 +8566,13 @@
       <c r="AT17" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="AU17" s="111" t="s">
+      <c r="AU17" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="AV17" s="112"/>
+      <c r="AV17" s="118"/>
     </row>
     <row r="18" spans="2:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="115"/>
+      <c r="B18" s="121"/>
       <c r="C18" s="20" t="s">
         <v>87</v>
       </c>
@@ -8594,7 +8714,7 @@
     </row>
     <row r="19" spans="2:48" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:48" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="114" t="s">
+      <c r="B20" s="120" t="s">
         <v>77</v>
       </c>
       <c r="C20" s="13" t="s">
@@ -8729,13 +8849,13 @@
       <c r="AT20" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="AU20" s="111" t="s">
+      <c r="AU20" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="AV20" s="112"/>
+      <c r="AV20" s="118"/>
     </row>
     <row r="21" spans="2:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="115"/>
+      <c r="B21" s="121"/>
       <c r="C21" s="20" t="s">
         <v>87</v>
       </c>
@@ -8921,7 +9041,7 @@
       <c r="AV22" s="7"/>
     </row>
     <row r="23" spans="2:48" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="114" t="s">
+      <c r="B23" s="120" t="s">
         <v>94</v>
       </c>
       <c r="C23" s="13" t="s">
@@ -8936,34 +9056,34 @@
       <c r="F23" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="G23" s="123" t="s">
+      <c r="G23" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="123"/>
-      <c r="I23" s="124" t="s">
+      <c r="H23" s="129"/>
+      <c r="I23" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="J23" s="124"/>
-      <c r="K23" s="119" t="s">
+      <c r="J23" s="130"/>
+      <c r="K23" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="L23" s="119"/>
-      <c r="M23" s="120" t="s">
+      <c r="L23" s="125"/>
+      <c r="M23" s="126" t="s">
         <v>33</v>
       </c>
-      <c r="N23" s="120"/>
-      <c r="O23" s="121" t="s">
+      <c r="N23" s="126"/>
+      <c r="O23" s="127" t="s">
         <v>34</v>
       </c>
-      <c r="P23" s="121"/>
-      <c r="Q23" s="118" t="s">
+      <c r="P23" s="127"/>
+      <c r="Q23" s="124" t="s">
         <v>35</v>
       </c>
-      <c r="R23" s="118"/>
-      <c r="S23" s="122" t="s">
+      <c r="R23" s="124"/>
+      <c r="S23" s="128" t="s">
         <v>36</v>
       </c>
-      <c r="T23" s="122"/>
+      <c r="T23" s="128"/>
       <c r="U23" s="10" t="s">
         <v>51</v>
       </c>
@@ -9042,13 +9162,13 @@
       <c r="AT23" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="AU23" s="111" t="s">
+      <c r="AU23" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="AV23" s="112"/>
+      <c r="AV23" s="118"/>
     </row>
     <row r="24" spans="2:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="115"/>
+      <c r="B24" s="121"/>
       <c r="C24" s="20" t="s">
         <v>87</v>
       </c>
@@ -9201,7 +9321,7 @@
       <c r="AV25" s="7"/>
     </row>
     <row r="26" spans="2:48" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="114" t="s">
+      <c r="B26" s="120" t="s">
         <v>95</v>
       </c>
       <c r="C26" s="13" t="s">
@@ -9216,62 +9336,62 @@
       <c r="F26" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="G26" s="116" t="s">
+      <c r="G26" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="117"/>
-      <c r="I26" s="116" t="s">
+      <c r="H26" s="123"/>
+      <c r="I26" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="J26" s="117"/>
-      <c r="K26" s="116" t="s">
+      <c r="J26" s="123"/>
+      <c r="K26" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="L26" s="117"/>
-      <c r="M26" s="116" t="s">
+      <c r="L26" s="123"/>
+      <c r="M26" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="N26" s="117"/>
-      <c r="O26" s="116" t="s">
+      <c r="N26" s="123"/>
+      <c r="O26" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="P26" s="117"/>
-      <c r="Q26" s="116" t="s">
+      <c r="P26" s="123"/>
+      <c r="Q26" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="R26" s="117"/>
-      <c r="S26" s="116" t="s">
+      <c r="R26" s="123"/>
+      <c r="S26" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="T26" s="117"/>
-      <c r="U26" s="116" t="s">
+      <c r="T26" s="123"/>
+      <c r="U26" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="V26" s="117"/>
-      <c r="W26" s="116" t="s">
+      <c r="V26" s="123"/>
+      <c r="W26" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="X26" s="117"/>
-      <c r="Y26" s="116" t="s">
+      <c r="X26" s="123"/>
+      <c r="Y26" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="Z26" s="117"/>
-      <c r="AA26" s="116" t="s">
+      <c r="Z26" s="123"/>
+      <c r="AA26" s="122" t="s">
         <v>22</v>
       </c>
-      <c r="AB26" s="117"/>
-      <c r="AC26" s="126" t="s">
+      <c r="AB26" s="123"/>
+      <c r="AC26" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="AD26" s="126"/>
-      <c r="AE26" s="126" t="s">
+      <c r="AD26" s="132"/>
+      <c r="AE26" s="132" t="s">
         <v>24</v>
       </c>
-      <c r="AF26" s="126"/>
-      <c r="AG26" s="126" t="s">
+      <c r="AF26" s="132"/>
+      <c r="AG26" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="AH26" s="126"/>
+      <c r="AH26" s="132"/>
       <c r="AI26" s="27" t="s">
         <v>65</v>
       </c>
@@ -9308,13 +9428,13 @@
       <c r="AT26" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="AU26" s="111" t="s">
+      <c r="AU26" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="AV26" s="112"/>
+      <c r="AV26" s="118"/>
     </row>
     <row r="27" spans="2:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="115"/>
+      <c r="B27" s="121"/>
       <c r="C27" s="20" t="s">
         <v>87</v>
       </c>
@@ -9466,7 +9586,7 @@
       <c r="AV28" s="7"/>
     </row>
     <row r="29" spans="2:48" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="114" t="s">
+      <c r="B29" s="120" t="s">
         <v>96</v>
       </c>
       <c r="C29" s="13" t="s">
@@ -9481,30 +9601,30 @@
       <c r="F29" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="G29" s="127" t="s">
+      <c r="G29" s="133" t="s">
         <v>27</v>
       </c>
-      <c r="H29" s="129"/>
-      <c r="I29" s="127" t="s">
+      <c r="H29" s="135"/>
+      <c r="I29" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="J29" s="129"/>
-      <c r="K29" s="127" t="s">
+      <c r="J29" s="135"/>
+      <c r="K29" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="L29" s="129"/>
-      <c r="M29" s="127" t="s">
+      <c r="L29" s="135"/>
+      <c r="M29" s="133" t="s">
         <v>30</v>
       </c>
-      <c r="N29" s="129"/>
-      <c r="O29" s="127" t="s">
+      <c r="N29" s="135"/>
+      <c r="O29" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="P29" s="129"/>
-      <c r="Q29" s="127" t="s">
+      <c r="P29" s="135"/>
+      <c r="Q29" s="133" t="s">
         <v>32</v>
       </c>
-      <c r="R29" s="128"/>
+      <c r="R29" s="134"/>
       <c r="S29" s="10" t="s">
         <v>49</v>
       </c>
@@ -9589,13 +9709,13 @@
       <c r="AT29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="AU29" s="111" t="s">
+      <c r="AU29" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="AV29" s="112"/>
+      <c r="AV29" s="118"/>
     </row>
     <row r="30" spans="2:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="115"/>
+      <c r="B30" s="121"/>
       <c r="C30" s="20" t="s">
         <v>87</v>
       </c>
@@ -9736,62 +9856,62 @@
       </c>
     </row>
     <row r="32" spans="2:48" x14ac:dyDescent="0.25">
-      <c r="G32" s="130" t="s">
+      <c r="G32" s="136" t="s">
         <v>101</v>
       </c>
-      <c r="H32" s="130"/>
-      <c r="I32" s="130" t="s">
+      <c r="H32" s="136"/>
+      <c r="I32" s="136" t="s">
         <v>102</v>
       </c>
-      <c r="J32" s="130"/>
-      <c r="K32" s="130" t="s">
+      <c r="J32" s="136"/>
+      <c r="K32" s="136" t="s">
         <v>103</v>
       </c>
-      <c r="L32" s="130"/>
-      <c r="M32" s="130" t="s">
+      <c r="L32" s="136"/>
+      <c r="M32" s="136" t="s">
         <v>104</v>
       </c>
-      <c r="N32" s="130"/>
-      <c r="O32" s="130" t="s">
+      <c r="N32" s="136"/>
+      <c r="O32" s="136" t="s">
         <v>105</v>
       </c>
-      <c r="P32" s="130"/>
-      <c r="Q32" s="130" t="s">
+      <c r="P32" s="136"/>
+      <c r="Q32" s="136" t="s">
         <v>106</v>
       </c>
-      <c r="R32" s="130"/>
-      <c r="S32" s="130" t="s">
+      <c r="R32" s="136"/>
+      <c r="S32" s="136" t="s">
         <v>107</v>
       </c>
-      <c r="T32" s="130"/>
-      <c r="U32" s="130" t="s">
+      <c r="T32" s="136"/>
+      <c r="U32" s="136" t="s">
         <v>108</v>
       </c>
-      <c r="V32" s="130"/>
-      <c r="W32" s="130" t="s">
+      <c r="V32" s="136"/>
+      <c r="W32" s="136" t="s">
         <v>109</v>
       </c>
-      <c r="X32" s="130"/>
-      <c r="Y32" s="130" t="s">
+      <c r="X32" s="136"/>
+      <c r="Y32" s="136" t="s">
         <v>110</v>
       </c>
-      <c r="Z32" s="130"/>
-      <c r="AA32" s="130" t="s">
+      <c r="Z32" s="136"/>
+      <c r="AA32" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="AB32" s="130"/>
-      <c r="AC32" s="130" t="s">
+      <c r="AB32" s="136"/>
+      <c r="AC32" s="136" t="s">
         <v>112</v>
       </c>
-      <c r="AD32" s="130"/>
-      <c r="AE32" s="130" t="s">
+      <c r="AD32" s="136"/>
+      <c r="AE32" s="136" t="s">
         <v>113</v>
       </c>
-      <c r="AF32" s="130"/>
-      <c r="AG32" s="130" t="s">
+      <c r="AF32" s="136"/>
+      <c r="AG32" s="136" t="s">
         <v>114</v>
       </c>
-      <c r="AH32" s="130"/>
+      <c r="AH32" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="60">

</xml_diff>